<commit_message>
📊 Horarios actualizados Línea 141 - 47
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 00:46:06</t>
+          <t>Última actualización: 01:22:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -517,6 +517,26 @@
       </c>
       <c r="D7" t="n">
         <v>72</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01:22:42</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -525,88 +545,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - LP1912-215 - 10/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 00:46:06</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>00:46:06</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>01:12</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -623,14 +561,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - 6203-6173 - 10/01/2026</t>
+          <t>LÍNEA 141 - LP1912-215 - 10/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 00:46:06</t>
+          <t>Última actualización: 01:22:42</t>
         </is>
       </c>
     </row>
@@ -686,6 +624,108 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>01:22:42</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - 6203-6173 - 10/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 01:22:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>00:46:06</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>01:12</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>00:46:06</t>
         </is>
       </c>
@@ -701,6 +741,26 @@
       </c>
       <c r="D7" t="n">
         <v>72</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01:22:42</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 48
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:22:42</t>
+          <t>Última actualización: 01:55:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -502,41 +502,81 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>00:46:06</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>01:58</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>01:22:42</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>02:58</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>215_ALUAR</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D9" t="n">
         <v>96</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -568,7 +608,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:22:42</t>
+          <t>Última actualización: 01:55:38</t>
         </is>
       </c>
     </row>
@@ -652,7 +692,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -670,14 +710,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:22:42</t>
+          <t>Última actualización: 01:55:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -726,41 +766,81 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>00:46:06</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>01:58</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>01:22:42</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>02:58</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>215_ALUAR</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D9" t="n">
         <v>96</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 49
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:55:38</t>
+          <t>Última actualización: 02:29:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -542,40 +542,60 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>01:22:42</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>01:55:38</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>03:48</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
         <v>113</v>
       </c>
     </row>
@@ -608,7 +628,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:55:38</t>
+          <t>Última actualización: 02:29:13</t>
         </is>
       </c>
     </row>
@@ -692,7 +712,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -710,14 +730,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:55:38</t>
+          <t>Última actualización: 02:29:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -806,40 +826,60 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>01:22:42</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>01:55:38</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>03:48</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
         <v>113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 50
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:29:13</t>
+          <t>Última actualización: 02:47:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -597,6 +597,26 @@
       </c>
       <c r="D11" t="n">
         <v>113</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>02:47:42</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -610,7 +630,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -628,14 +648,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:29:13</t>
+          <t>Última actualización: 02:47:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -699,6 +719,26 @@
       </c>
       <c r="D7" t="n">
         <v>96</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>02:47:42</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -712,7 +752,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -730,14 +770,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:29:13</t>
+          <t>Última actualización: 02:47:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -881,6 +921,26 @@
       </c>
       <c r="D11" t="n">
         <v>113</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>02:47:42</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 51
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:47:42</t>
+          <t>Última actualización: 03:00:53</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -602,20 +602,40 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D13" t="n">
         <v>118</v>
       </c>
     </row>
@@ -648,7 +668,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:47:42</t>
+          <t>Última actualización: 03:00:53</t>
         </is>
       </c>
     </row>
@@ -752,7 +772,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -770,14 +790,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:47:42</t>
+          <t>Última actualización: 03:00:53</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -926,20 +946,40 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D13" t="n">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 52
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:00:53</t>
+          <t>Última actualización: 03:46:12</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -502,140 +502,220 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>05:22</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D17" t="n">
         <v>118</v>
       </c>
     </row>
@@ -650,7 +730,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -668,14 +748,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:00:53</t>
+          <t>Última actualización: 03:46:12</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -724,40 +804,80 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>96</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>01:22:42</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D10" t="n">
         <v>118</v>
       </c>
     </row>
@@ -772,7 +892,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -790,14 +910,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:00:53</t>
+          <t>Última actualización: 03:46:12</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -846,140 +966,220 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>05:22</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D17" t="n">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 53
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:46:12</t>
+          <t>Última actualización: 04:01:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 18</t>
         </is>
       </c>
     </row>
@@ -482,141 +482,141 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01:12</t>
+          <t>04:02</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>01:12</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>60</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>90</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>96</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13">
@@ -627,95 +627,215 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>01:22:42</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>05:45</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>05:52</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D23" t="n">
         <v>118</v>
       </c>
     </row>
@@ -730,7 +850,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -748,14 +868,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:46:12</t>
+          <t>Última actualización: 04:01:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -804,80 +924,100 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>96</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
         <v>118</v>
       </c>
     </row>
@@ -892,7 +1032,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -910,14 +1050,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:46:12</t>
+          <t>Última actualización: 04:01:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 18</t>
         </is>
       </c>
     </row>
@@ -946,141 +1086,141 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01:12</t>
+          <t>04:02</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>01:12</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>60</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>90</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>96</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13">
@@ -1091,95 +1231,215 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>01:22:42</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>05:45</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>05:52</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D23" t="n">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 54
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:01:06</t>
+          <t>Última actualización: 04:30:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 18</t>
+          <t>Total filas: 24</t>
         </is>
       </c>
     </row>
@@ -622,52 +622,52 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -676,67 +676,67 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19">
@@ -747,95 +747,215 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>05:52</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>06:24</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D29" t="n">
         <v>118</v>
       </c>
     </row>
@@ -850,7 +970,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -868,14 +988,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:01:06</t>
+          <t>Última actualización: 04:30:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -984,40 +1104,60 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D12" t="n">
         <v>118</v>
       </c>
     </row>
@@ -1032,7 +1172,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1050,14 +1190,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:01:06</t>
+          <t>Última actualización: 04:30:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 18</t>
+          <t>Total filas: 24</t>
         </is>
       </c>
     </row>
@@ -1226,52 +1366,52 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1280,67 +1420,67 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19">
@@ -1351,95 +1491,215 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>05:52</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>06:24</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D29" t="n">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 55
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:30:03</t>
+          <t>Última actualización: 04:44:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 24</t>
+          <t>Total filas: 38</t>
         </is>
       </c>
     </row>
@@ -502,81 +502,81 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>01:12</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>01:12</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>05:11</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>60</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>05:21</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11">
@@ -587,47 +587,47 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>71</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>05:31</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -636,7 +636,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
@@ -647,176 +647,176 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>91</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>05:51</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>91</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>94</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>06:03</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>101</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23">
@@ -827,76 +827,76 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>113</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27">
@@ -907,55 +907,335 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>114</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>05:22</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>06:23</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>06:26</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>05:45</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>06:30</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>06:30</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>05:52</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>06:24</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>06:38</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B43" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="D43" t="n">
         <v>118</v>
       </c>
     </row>
@@ -970,7 +1250,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -988,14 +1268,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:30:03</t>
+          <t>Última actualización: 04:44:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 9</t>
         </is>
       </c>
     </row>
@@ -1024,92 +1304,92 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01:12</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>01:12</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>96</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1118,46 +1398,86 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D14" t="n">
         <v>118</v>
       </c>
     </row>
@@ -1172,7 +1492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1190,14 +1510,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:30:03</t>
+          <t>Última actualización: 04:44:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 24</t>
+          <t>Total filas: 38</t>
         </is>
       </c>
     </row>
@@ -1246,81 +1566,81 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>01:12</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>01:12</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>05:11</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>60</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>05:21</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11">
@@ -1331,47 +1651,47 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>71</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>05:31</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1380,7 +1700,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
@@ -1391,176 +1711,176 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>91</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>05:51</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>91</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>94</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>06:03</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>101</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23">
@@ -1571,76 +1891,76 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>113</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27">
@@ -1651,55 +1971,335 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>114</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>05:22</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>06:23</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>06:26</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>05:45</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>06:30</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>06:30</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>05:52</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>06:24</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>06:38</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B43" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="D43" t="n">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 56
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:44:55</t>
+          <t>Última actualización: 04:58:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 38</t>
+          <t>Total filas: 44</t>
         </is>
       </c>
     </row>
@@ -502,61 +502,61 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>04:59</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>01:12</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05:11</t>
+          <t>01:12</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
@@ -567,56 +567,56 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:21</t>
+          <t>05:11</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>05:21</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>05:31</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
@@ -627,56 +627,56 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:43</t>
+          <t>05:31</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16">
@@ -702,52 +702,52 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -756,27 +756,27 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21">
@@ -787,16 +787,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>06:03</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22">
@@ -807,72 +807,72 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>06:03</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -882,12 +882,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -896,118 +896,118 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>06:23</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1016,87 +1016,87 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>06:23</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37">
@@ -1107,135 +1107,255 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>06:38</t>
+          <t>05:52</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>06:51</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>06:38</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>06:24</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B49" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D43" t="n">
+      <c r="D49" t="n">
         <v>118</v>
       </c>
     </row>
@@ -1250,7 +1370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1268,14 +1388,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:44:55</t>
+          <t>Última actualización: 04:58:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 9</t>
+          <t>Total filas: 10</t>
         </is>
       </c>
     </row>
@@ -1464,20 +1584,40 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>06:51</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D15" t="n">
         <v>118</v>
       </c>
     </row>
@@ -1492,7 +1632,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1510,14 +1650,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:44:55</t>
+          <t>Última actualización: 04:58:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 38</t>
+          <t>Total filas: 44</t>
         </is>
       </c>
     </row>
@@ -1566,61 +1706,61 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>04:59</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>01:12</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05:11</t>
+          <t>01:12</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
@@ -1631,56 +1771,56 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:21</t>
+          <t>05:11</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>05:21</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>05:31</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
@@ -1691,56 +1831,56 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:43</t>
+          <t>05:31</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16">
@@ -1766,52 +1906,52 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1820,27 +1960,27 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21">
@@ -1851,16 +1991,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>06:03</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22">
@@ -1871,72 +2011,72 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>06:03</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1946,12 +2086,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1960,118 +2100,118 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>06:23</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2080,87 +2220,87 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>06:23</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37">
@@ -2171,135 +2311,255 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>06:38</t>
+          <t>05:52</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>06:51</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>06:38</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>06:24</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B49" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D43" t="n">
+      <c r="D49" t="n">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 57
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:58:02</t>
+          <t>Última actualización: 05:37:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 44</t>
+          <t>Total filas: 51</t>
         </is>
       </c>
     </row>
@@ -822,132 +822,132 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -956,227 +956,227 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>06:23</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>07:14</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>06:23</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41">
@@ -1187,175 +1187,315 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>06:38</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>07:27</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>06:54</t>
+          <t>05:52</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:51</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>06:38</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>06:24</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>07:33</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B56" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D49" t="n">
+      <c r="D56" t="n">
         <v>118</v>
       </c>
     </row>
@@ -1370,7 +1510,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1388,14 +1528,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:58:02</t>
+          <t>Última actualización: 05:37:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 10</t>
+          <t>Total filas: 13</t>
         </is>
       </c>
     </row>
@@ -1524,72 +1664,72 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1598,26 +1738,86 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>07:27</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>06:51</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="D18" t="n">
         <v>118</v>
       </c>
     </row>
@@ -1632,7 +1832,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1650,14 +1850,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:58:02</t>
+          <t>Última actualización: 05:37:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 44</t>
+          <t>Total filas: 51</t>
         </is>
       </c>
     </row>
@@ -2026,132 +2226,132 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2160,227 +2360,227 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>06:23</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>07:14</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>06:23</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41">
@@ -2391,175 +2591,315 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>06:38</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>07:27</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>06:54</t>
+          <t>05:52</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:51</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>06:38</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>06:24</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>07:33</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B56" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D49" t="n">
+      <c r="D56" t="n">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 58
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:37:13</t>
+          <t>Última actualización: 05:55:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 51</t>
+          <t>Total filas: 62</t>
         </is>
       </c>
     </row>
@@ -642,41 +642,41 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>05:43</t>
+          <t>06:50</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>06:53</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16">
@@ -687,267 +687,267 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>05:51</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>05:51</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>07:03</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>06:03</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:01</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>07:04</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:13</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>06:03</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -956,187 +956,187 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>07:14</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>06:23</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>07:28</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39">
@@ -1147,96 +1147,96 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>07:14</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44">
@@ -1247,255 +1247,475 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:23</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>07:27</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>06:38</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>06:54</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:33</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>07:27</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>05:52</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>06:51</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>06:38</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>06:24</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>07:33</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>05:55:51</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B67" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C67" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D56" t="n">
+      <c r="D67" t="n">
         <v>118</v>
       </c>
     </row>
@@ -1510,7 +1730,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1528,14 +1748,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:37:13</t>
+          <t>Última actualización: 05:55:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 13</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -1624,12 +1844,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>06:50</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1638,18 +1858,18 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1658,18 +1878,18 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>86</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1678,87 +1898,87 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16">
@@ -1769,55 +1989,95 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>07:27</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>07:27</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>06:51</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D20" t="n">
         <v>118</v>
       </c>
     </row>
@@ -1832,7 +2092,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1850,14 +2110,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:37:13</t>
+          <t>Última actualización: 05:55:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 51</t>
+          <t>Total filas: 62</t>
         </is>
       </c>
     </row>
@@ -2046,41 +2306,41 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>05:43</t>
+          <t>06:50</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>06:53</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16">
@@ -2091,267 +2351,267 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>05:51</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>05:51</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>07:03</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>06:03</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:01</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>07:04</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:13</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>06:03</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2360,187 +2620,187 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>07:14</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>06:23</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>07:28</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39">
@@ -2551,96 +2811,96 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>07:14</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44">
@@ -2651,255 +2911,475 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:23</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>07:27</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>06:38</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>06:54</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:33</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>07:27</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>05:52</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>06:51</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>06:38</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>06:24</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>07:33</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>05:55:51</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B67" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C67" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D56" t="n">
+      <c r="D67" t="n">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 59
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:55:52</t>
+          <t>Última actualización: 06:28:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 62</t>
+          <t>Total filas: 76</t>
         </is>
       </c>
     </row>
@@ -482,37 +482,37 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:02</t>
+          <t>06:28</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:59</t>
+          <t>04:02</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -522,101 +522,101 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>04:59</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>01:12</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:11</t>
+          <t>06:32</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:21</t>
+          <t>01:12</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>05:11</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13">
@@ -627,87 +627,87 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:31</t>
+          <t>05:21</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:50</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:53</t>
+          <t>05:31</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>05:43</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>06:50</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -716,7 +716,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18">
@@ -727,16 +727,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>06:53</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19">
@@ -747,76 +747,76 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:51</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>07:03</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23">
@@ -827,76 +827,76 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:06</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>05:51</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27">
@@ -907,167 +907,167 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>07:13</t>
+          <t>07:03</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>06:03</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>07:01</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>07:04</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:13</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>06:03</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1076,198 +1076,198 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>07:28</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>07:58</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>07:59</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>07:14</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>06:23</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1276,27 +1276,27 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>07:28</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47">
@@ -1307,116 +1307,116 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>07:14</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53">
@@ -1427,16 +1427,16 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:23</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54">
@@ -1447,275 +1447,555 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>08:09</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>07:27</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>08:10</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>06:38</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>06:54</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>07:33</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>08:15</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>07:27</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>05:52</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>06:51</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>06:38</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>06:24</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>06:28:32</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>05:55:51</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>07:33</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
+      <c r="B80" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D67" t="n">
+      <c r="D80" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>06:28:32</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>08:26</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
         <v>118</v>
       </c>
     </row>
@@ -1730,7 +2010,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1748,14 +2028,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:55:52</t>
+          <t>Última actualización: 06:28:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 18</t>
         </is>
       </c>
     </row>
@@ -1884,112 +2164,112 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>07:06</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1998,27 +2278,27 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>08:10</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18">
@@ -2029,55 +2309,115 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>07:27</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>07:27</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>06:51</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>06:28:32</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D23" t="n">
         <v>118</v>
       </c>
     </row>
@@ -2092,7 +2432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2110,14 +2450,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:55:52</t>
+          <t>Última actualización: 06:28:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 62</t>
+          <t>Total filas: 76</t>
         </is>
       </c>
     </row>
@@ -2146,37 +2486,37 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:02</t>
+          <t>06:28</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:59</t>
+          <t>04:02</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -2186,101 +2526,101 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>04:59</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>01:12</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:11</t>
+          <t>06:32</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:21</t>
+          <t>01:12</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>05:11</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13">
@@ -2291,87 +2631,87 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:31</t>
+          <t>05:21</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:50</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:53</t>
+          <t>05:31</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>05:43</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>06:50</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2380,7 +2720,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18">
@@ -2391,16 +2731,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>06:53</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19">
@@ -2411,76 +2751,76 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:51</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>07:03</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23">
@@ -2491,76 +2831,76 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:06</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>05:51</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27">
@@ -2571,167 +2911,167 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>07:13</t>
+          <t>07:03</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>06:03</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>07:01</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>07:04</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:13</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>06:03</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2740,198 +3080,198 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>07:28</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>07:58</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>07:59</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>07:14</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>06:23</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2940,27 +3280,27 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>07:28</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47">
@@ -2971,116 +3311,116 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>07:14</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53">
@@ -3091,16 +3431,16 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:23</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54">
@@ -3111,275 +3451,555 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>08:09</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>07:27</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>08:10</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>06:38</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>06:54</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>07:33</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>08:15</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
+          <t>03:46:12</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>07:27</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>04:01:06</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>05:52</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>06:51</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>03:00:53</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>01:55:38</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>04:44:55</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>06:38</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>06:24</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>06:28:32</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>05:55:51</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>07:33</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
+      <c r="B80" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D67" t="n">
+      <c r="D80" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>06:28:32</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>08:26</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 60
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:28:32</t>
+          <t>Última actualización: 06:45:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 76</t>
+          <t>Total filas: 82</t>
         </is>
       </c>
     </row>
@@ -642,81 +642,81 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>07:28</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>05:31</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>05:31</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06:50</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18">
@@ -727,27 +727,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06:53</t>
+          <t>06:50</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:43</t>
+          <t>06:53</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -756,47 +756,47 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22">
@@ -822,57 +822,57 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>05:51</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -882,37 +882,37 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>05:51</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>07:03</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -922,37 +922,37 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>07:03</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>07:06</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -962,32 +962,32 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -996,87 +996,87 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>07:13</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>06:03</t>
+          <t>08:02</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>07:01</t>
+          <t>07:13</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36">
@@ -1087,16 +1087,16 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>06:03</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37">
@@ -1107,36 +1107,36 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>07:04</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39">
@@ -1147,32 +1147,32 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>07:58</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1182,41 +1182,41 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>07:59</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>07:58</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43">
@@ -1242,12 +1242,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1256,47 +1256,47 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>07:59</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>07:28</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47">
@@ -1322,197 +1322,197 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>07:28</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>08:03</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>07:14</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>06:23</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>07:14</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>08:09</t>
+          <t>06:23</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>08:09</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1542,212 +1542,212 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>08:10</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>08:10</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>08:29</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>08:31</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>07:27</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>08:15</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1756,138 +1756,138 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>07:27</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>06:38</t>
+          <t>05:52</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>06:51</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>03:00:53</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>06:54</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1896,107 +1896,227 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>06:38</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>07:33</t>
+          <t>06:24</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>08:39</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>02:47:42</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>04:45</t>
+          <t>08:23</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
+          <t>05:55:51</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>07:33</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
           <t>06:28:32</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="B85" t="inlineStr">
         <is>
           <t>08:26</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="C85" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D81" t="n">
+      <c r="D85" t="n">
         <v>118</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>02:47:42</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>06:45:29</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2010,7 +2130,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2028,14 +2148,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:28:32</t>
+          <t>Última actualización: 06:45:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 18</t>
+          <t>Total filas: 20</t>
         </is>
       </c>
     </row>
@@ -2104,52 +2224,52 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>07:28</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>06:50</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>06:50</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2158,266 +2278,306 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>07:06</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>08:10</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>08:10</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>07:27</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>07:27</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>06:51</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>06:45:29</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>08:39</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>06:28:32</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D25" t="n">
         <v>118</v>
       </c>
     </row>
@@ -2432,7 +2592,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2450,14 +2610,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:28:32</t>
+          <t>Última actualización: 06:45:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 76</t>
+          <t>Total filas: 82</t>
         </is>
       </c>
     </row>
@@ -2646,81 +2806,81 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>07:28</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>05:31</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>05:31</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06:50</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18">
@@ -2731,27 +2891,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06:53</t>
+          <t>06:50</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:43</t>
+          <t>06:53</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2760,47 +2920,47 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22">
@@ -2826,57 +2986,57 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>05:51</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -2886,37 +3046,37 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>05:51</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>07:03</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -2926,37 +3086,37 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>07:03</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>07:06</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -2966,32 +3126,32 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -3000,87 +3160,87 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>07:13</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>06:03</t>
+          <t>08:02</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>07:01</t>
+          <t>07:13</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36">
@@ -3091,16 +3251,16 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>06:03</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37">
@@ -3111,36 +3271,36 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>07:04</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39">
@@ -3151,32 +3311,32 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>07:58</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -3186,41 +3346,41 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>07:59</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>07:58</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43">
@@ -3246,12 +3406,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -3260,47 +3420,47 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>07:59</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>07:28</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47">
@@ -3326,197 +3486,197 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>07:28</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>08:03</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>07:14</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>06:23</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>07:14</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>08:09</t>
+          <t>06:23</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>08:09</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -3546,212 +3706,212 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>08:10</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>08:10</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>08:29</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>08:31</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>07:27</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>08:15</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3760,138 +3920,138 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>07:27</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>06:38</t>
+          <t>05:52</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>06:51</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>03:00:53</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>06:54</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3900,107 +4060,227 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>06:38</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>07:33</t>
+          <t>06:24</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>08:39</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>02:47:42</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>04:45</t>
+          <t>08:23</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
+          <t>05:55:51</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>07:33</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
           <t>06:28:32</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="B85" t="inlineStr">
         <is>
           <t>08:26</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="C85" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D81" t="n">
+      <c r="D85" t="n">
         <v>118</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>02:47:42</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>06:45:29</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 61
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:45:29</t>
+          <t>Última actualización: 06:58:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 82</t>
+          <t>Total filas: 90</t>
         </is>
       </c>
     </row>
@@ -622,12 +622,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:21</t>
+          <t>07:34</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -636,287 +636,287 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>06:45:29</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>07:28</t>
+          <t>05:21</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>05:31</t>
+          <t>07:28</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06:50</t>
+          <t>05:31</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>06:53</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>05:43</t>
+          <t>06:50</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>06:53</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>05:51</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>08:01</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28">
@@ -927,196 +927,196 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>07:03</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>07:06</t>
+          <t>05:51</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>07:03</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:45:29</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>08:02</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>07:13</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>06:03</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>07:01</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38">
@@ -1127,376 +1127,376 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>07:04</t>
+          <t>08:02</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>07:13</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>06:03</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>07:58</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>07:59</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>07:58</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>07:28</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>07:59</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>08:03</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>08:30</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:14</t>
+          <t>07:28</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>06:23</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57">
@@ -1507,76 +1507,76 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>08:09</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>07:14</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61">
@@ -1587,116 +1587,116 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>06:23</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>08:10</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>06:45:29</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>08:29</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>08:09</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>06:45:29</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>08:31</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67">
@@ -1707,336 +1707,336 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>08:10</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>08:29</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>07:27</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>08:31</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>08:15</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>06:38</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>07:27</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>06:45:29</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>08:39</t>
+          <t>05:52</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>06:51</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>07:33</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>03:00:53</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>06:54</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84">
@@ -2047,75 +2047,235 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:24</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>08:26</t>
+          <t>06:38</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>02:47:42</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>04:45</t>
+          <t>08:39</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
+          <t>06:58:06</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>08:52</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>06:28:32</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>05:55:51</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>07:33</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>06:28:32</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>08:26</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>02:47:42</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
           <t>06:45:29</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B95" t="inlineStr">
         <is>
           <t>08:44</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="C95" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D87" t="n">
+      <c r="D95" t="n">
         <v>119</v>
       </c>
     </row>
@@ -2130,7 +2290,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2148,14 +2308,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:45:29</t>
+          <t>Última actualización: 06:58:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 20</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -2504,12 +2664,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2518,66 +2678,106 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:45:29</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>08:39</t>
+          <t>06:51</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>06:45:29</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>08:39</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>06:28:32</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>02:47:42</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>04:45</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D25" t="n">
+      <c r="D27" t="n">
         <v>118</v>
       </c>
     </row>
@@ -2592,7 +2792,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2610,14 +2810,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:45:29</t>
+          <t>Última actualización: 06:58:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 82</t>
+          <t>Total filas: 90</t>
         </is>
       </c>
     </row>
@@ -2786,12 +2986,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:21</t>
+          <t>07:34</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2800,287 +3000,287 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>06:45:29</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>07:28</t>
+          <t>05:21</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>05:31</t>
+          <t>07:28</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06:50</t>
+          <t>05:31</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>06:53</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>05:43</t>
+          <t>06:50</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>06:53</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>05:51</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>08:01</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28">
@@ -3091,196 +3291,196 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>07:03</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>07:06</t>
+          <t>05:51</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>00:46:06</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>07:03</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:45:29</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>08:02</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>07:13</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>00:46:06</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>06:03</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>07:01</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38">
@@ -3291,376 +3491,376 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>06:10</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>07:04</t>
+          <t>08:02</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>07:13</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>06:03</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>07:58</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>06:10</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>07:59</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>02:29:13</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>07:58</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>07:28</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>07:59</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>02:29:13</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>08:03</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>01:22:42</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>08:30</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:14</t>
+          <t>07:28</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>06:23</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57">
@@ -3671,76 +3871,76 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>08:09</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>01:22:42</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>07:14</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61">
@@ -3751,116 +3951,116 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>06:23</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>08:10</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>06:45:29</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>08:29</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>05:45</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>08:09</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>06:45:29</t>
+          <t>04:30:03</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>08:31</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67">
@@ -3871,336 +4071,336 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>08:10</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>08:29</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>05:45</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>07:27</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>04:01:06</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>08:31</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>06:51</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>03:00:53</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>08:15</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>01:55:38</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>06:38</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>04:30:03</t>
+          <t>05:37:13</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>07:27</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>06:45:29</t>
+          <t>04:01:06</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>08:39</t>
+          <t>05:52</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>04:58:02</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>06:51</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>05:37:13</t>
+          <t>01:55:38</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>07:33</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>04:58:02</t>
+          <t>03:00:53</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>06:54</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84">
@@ -4211,75 +4411,235 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:24</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>08:26</t>
+          <t>06:38</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>02:47:42</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>04:45</t>
+          <t>08:39</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
+          <t>06:58:06</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>08:52</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>06:28:32</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>05:55:51</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>04:58:02</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>05:37:13</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>07:33</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>06:28:32</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>08:26</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>02:47:42</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
           <t>06:45:29</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B95" t="inlineStr">
         <is>
           <t>08:44</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="C95" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D87" t="n">
+      <c r="D95" t="n">
         <v>119</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 76
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E250"/>
+  <dimension ref="A1:E254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:41:18</t>
+          <t>Última actualización: 12:46:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 245</t>
+          <t>Total filas: 249</t>
         </is>
       </c>
     </row>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -2786,7 +2786,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -4036,7 +4036,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>10:51:31</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4046,18 +4046,18 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>10:51:31</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4067,11 +4067,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E176" t="inlineStr"/>
     </row>
@@ -4372,7 +4372,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -4382,18 +4382,18 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="E191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -4403,11 +4403,11 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="E192" t="inlineStr"/>
     </row>
@@ -5346,12 +5346,12 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>13:39</t>
+          <t>13:38</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -5360,93 +5360,101 @@
         </is>
       </c>
       <c r="D237" t="n">
-        <v>70</v>
-      </c>
-      <c r="E237" t="inlineStr"/>
+        <v>52</v>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>13:40</t>
+          <t>13:39</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="E238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>13:42</t>
+          <t>13:40</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="E239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:42</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="E240" t="inlineStr"/>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>13:53</t>
+          <t>13:43</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>115</v>
-      </c>
-      <c r="E241" t="inlineStr"/>
+        <v>57</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -5456,28 +5464,28 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:51</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:53</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -5486,28 +5494,28 @@
         </is>
       </c>
       <c r="D243" t="n">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="E243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="E244" t="inlineStr"/>
     </row>
@@ -5519,43 +5527,39 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="E245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>12:38:18</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>103</v>
-      </c>
-      <c r="E246" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -5565,37 +5569,37 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>14:24</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:38:18</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>14:25</t>
+          <t>14:21</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -5606,27 +5610,23 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>14:37</t>
+          <t>14:24</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>116</v>
-      </c>
-      <c r="E249" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -5636,18 +5636,118 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
+          <t>14:25</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>104</v>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>12:46:01</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>108</v>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>14:37</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>116</v>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
           <t>14:40</t>
         </is>
       </c>
-      <c r="C250" t="inlineStr">
+      <c r="C253" t="inlineStr">
         <is>
           <t>17X38_ROMERO</t>
         </is>
       </c>
-      <c r="D250" t="n">
+      <c r="D253" t="n">
         <v>119</v>
       </c>
-      <c r="E250" t="inlineStr">
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>12:46:01</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>119</v>
+      </c>
+      <c r="E254" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5664,7 +5764,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5682,14 +5782,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:41:18</t>
+          <t>Última actualización: 12:46:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 65</t>
+          <t>Total filas: 67</t>
         </is>
       </c>
     </row>
@@ -7084,6 +7184,56 @@
         <v>103</v>
       </c>
       <c r="E70" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>12:46:01</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>108</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>12:46:01</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>119</v>
+      </c>
+      <c r="E72" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7100,7 +7250,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E250"/>
+  <dimension ref="A1:E254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7118,14 +7268,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:41:18</t>
+          <t>Última actualización: 12:46:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 245</t>
+          <t>Total filas: 249</t>
         </is>
       </c>
     </row>
@@ -8450,7 +8600,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -8471,7 +8621,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -9437,7 +9587,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -9458,7 +9608,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -10708,7 +10858,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>10:51:31</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -10718,18 +10868,18 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>10:51:31</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -10739,11 +10889,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E176" t="inlineStr"/>
     </row>
@@ -11044,7 +11194,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -11054,18 +11204,18 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="E191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -11075,11 +11225,11 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="E192" t="inlineStr"/>
     </row>
@@ -12018,12 +12168,12 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>13:39</t>
+          <t>13:38</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -12032,93 +12182,101 @@
         </is>
       </c>
       <c r="D237" t="n">
-        <v>70</v>
-      </c>
-      <c r="E237" t="inlineStr"/>
+        <v>52</v>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>13:40</t>
+          <t>13:39</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="E238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>13:42</t>
+          <t>13:40</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="E239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:42</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="E240" t="inlineStr"/>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>13:53</t>
+          <t>13:43</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>115</v>
-      </c>
-      <c r="E241" t="inlineStr"/>
+        <v>57</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -12128,28 +12286,28 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:51</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:53</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -12158,28 +12316,28 @@
         </is>
       </c>
       <c r="D243" t="n">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="E243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="E244" t="inlineStr"/>
     </row>
@@ -12191,43 +12349,39 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="E245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>12:38:18</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>103</v>
-      </c>
-      <c r="E246" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -12237,37 +12391,37 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>14:24</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:38:18</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>14:25</t>
+          <t>14:21</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -12278,27 +12432,23 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>14:37</t>
+          <t>14:24</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>116</v>
-      </c>
-      <c r="E249" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -12308,18 +12458,118 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
+          <t>14:25</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>104</v>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>12:46:01</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>108</v>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>14:37</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>116</v>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
           <t>14:40</t>
         </is>
       </c>
-      <c r="C250" t="inlineStr">
+      <c r="C253" t="inlineStr">
         <is>
           <t>17X38_ROMERO</t>
         </is>
       </c>
-      <c r="D250" t="n">
+      <c r="D253" t="n">
         <v>119</v>
       </c>
-      <c r="E250" t="inlineStr">
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>12:46:01</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>119</v>
+      </c>
+      <c r="E254" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 77
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E254"/>
+  <dimension ref="A1:E264"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:46:01</t>
+          <t>Última actualización: 12:58:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 249</t>
+          <t>Total filas: 259</t>
         </is>
       </c>
     </row>
@@ -2146,7 +2146,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2156,18 +2156,18 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>06:58:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2177,11 +2177,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="E86" t="inlineStr"/>
     </row>
@@ -3175,7 +3175,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>08:57:53</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3185,18 +3185,18 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="E134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>08:57:53</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3206,11 +3206,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E135" t="inlineStr"/>
     </row>
@@ -4183,7 +4183,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4193,18 +4193,18 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -4214,11 +4214,11 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E183" t="inlineStr"/>
     </row>
@@ -4943,33 +4943,37 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>13:01</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>34</v>
-      </c>
-      <c r="E218" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>12:38:18</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -4978,23 +4982,19 @@
         </is>
       </c>
       <c r="D219" t="n">
-        <v>26</v>
-      </c>
-      <c r="E219" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:38:18</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>13:05</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -5003,35 +5003,39 @@
         </is>
       </c>
       <c r="D220" t="n">
-        <v>80</v>
-      </c>
-      <c r="E220" t="inlineStr"/>
+        <v>26</v>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>13:05</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="E221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -5041,65 +5045,65 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="E223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>13:08</t>
+          <t>13:07</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="E224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>13:09</t>
+          <t>13:08</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -5108,56 +5112,56 @@
         </is>
       </c>
       <c r="D225" t="n">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="E225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>13:10</t>
+          <t>13:09</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="E226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>13:11</t>
+          <t>13:10</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>42</v>
+        <v>105</v>
       </c>
       <c r="E227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -5167,44 +5171,44 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="E228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:11</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="E229" t="inlineStr"/>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -5213,40 +5217,40 @@
         </is>
       </c>
       <c r="D230" t="n">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="E230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>13:18</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="E231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>13:19</t>
+          <t>13:18</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -5255,72 +5259,76 @@
         </is>
       </c>
       <c r="D232" t="n">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="E232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:19</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="E233" t="inlineStr"/>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="E234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>105</v>
-      </c>
-      <c r="E235" t="inlineStr"/>
+        <v>23</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -5330,282 +5338,282 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>13:31</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>13:38</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>52</v>
-      </c>
-      <c r="E237" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="E237" t="inlineStr"/>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>13:39</t>
+          <t>13:31</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="E238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>13:40</t>
+          <t>13:33</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>115</v>
-      </c>
-      <c r="E239" t="inlineStr"/>
+        <v>35</v>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>13:42</t>
+          <t>13:38</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>73</v>
-      </c>
-      <c r="E240" t="inlineStr"/>
+        <v>52</v>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>13:43</t>
+          <t>13:39</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>57</v>
-      </c>
-      <c r="E241" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:40</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>13:53</t>
+          <t>13:42</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="E243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:43</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>116</v>
-      </c>
-      <c r="E244" t="inlineStr"/>
+        <v>57</v>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:51</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="E245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:53</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="E246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="E247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>12:38:18</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>103</v>
-      </c>
-      <c r="E248" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -5615,37 +5623,37 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>14:24</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="E249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>14:25</t>
+          <t>14:11</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -5656,21 +5664,21 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -5681,46 +5689,42 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>14:37</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>116</v>
-      </c>
-      <c r="E252" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>14:40</t>
+          <t>14:20</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -5731,23 +5735,269 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
+          <t>12:38:18</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>103</v>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>12:29:23</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>14:24</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>115</v>
+      </c>
+      <c r="E255" t="inlineStr"/>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>14:25</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>104</v>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>95</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
           <t>12:46:01</t>
         </is>
       </c>
-      <c r="B254" t="inlineStr">
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>108</v>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>14:37</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>116</v>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>14:40</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D260" t="n">
+        <v>119</v>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>106</v>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>12:46:01</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
         <is>
           <t>14:45</t>
         </is>
       </c>
-      <c r="C254" t="inlineStr">
+      <c r="C262" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D254" t="n">
+      <c r="D262" t="n">
         <v>119</v>
       </c>
-      <c r="E254" t="inlineStr">
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D263" t="n">
+        <v>115</v>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>115</v>
+      </c>
+      <c r="E264" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5764,7 +6014,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5782,14 +6032,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:46:01</t>
+          <t>Última actualización: 12:58:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 67</t>
+          <t>Total filas: 71</t>
         </is>
       </c>
     </row>
@@ -6747,7 +6997,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -6757,18 +7007,18 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -6778,11 +7028,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E51" t="inlineStr"/>
     </row>
@@ -7167,12 +7417,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>12:38:18</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:20</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -7181,7 +7431,7 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -7192,21 +7442,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:38:18</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:21</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -7217,23 +7467,123 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>95</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
           <t>12:46:01</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>108</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>106</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>12:46:01</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
         <is>
           <t>14:45</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="C75" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D72" t="n">
+      <c r="D75" t="n">
         <v>119</v>
       </c>
-      <c r="E72" t="inlineStr">
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>115</v>
+      </c>
+      <c r="E76" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7250,7 +7600,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E254"/>
+  <dimension ref="A1:E264"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7268,14 +7618,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:46:01</t>
+          <t>Última actualización: 12:58:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 249</t>
+          <t>Total filas: 259</t>
         </is>
       </c>
     </row>
@@ -8968,7 +9318,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -8978,18 +9328,18 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>06:58:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -8999,11 +9349,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="E86" t="inlineStr"/>
     </row>
@@ -9997,7 +10347,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>08:57:53</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -10007,18 +10357,18 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="E134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>08:57:53</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -10028,11 +10378,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E135" t="inlineStr"/>
     </row>
@@ -11005,7 +11355,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -11015,18 +11365,18 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -11036,11 +11386,11 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E183" t="inlineStr"/>
     </row>
@@ -11765,33 +12115,37 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>13:01</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>34</v>
-      </c>
-      <c r="E218" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>12:38:18</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -11800,23 +12154,19 @@
         </is>
       </c>
       <c r="D219" t="n">
-        <v>26</v>
-      </c>
-      <c r="E219" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:38:18</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>13:05</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -11825,35 +12175,39 @@
         </is>
       </c>
       <c r="D220" t="n">
-        <v>80</v>
-      </c>
-      <c r="E220" t="inlineStr"/>
+        <v>26</v>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>13:05</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="E221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -11863,65 +12217,65 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="E223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>13:08</t>
+          <t>13:07</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="E224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>13:09</t>
+          <t>13:08</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -11930,56 +12284,56 @@
         </is>
       </c>
       <c r="D225" t="n">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="E225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>13:10</t>
+          <t>13:09</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="E226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>13:11</t>
+          <t>13:10</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>42</v>
+        <v>105</v>
       </c>
       <c r="E227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -11989,44 +12343,44 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="E228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:11</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="E229" t="inlineStr"/>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -12035,40 +12389,40 @@
         </is>
       </c>
       <c r="D230" t="n">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="E230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>13:18</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="E231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>13:19</t>
+          <t>13:18</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -12077,72 +12431,76 @@
         </is>
       </c>
       <c r="D232" t="n">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="E232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:19</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="E233" t="inlineStr"/>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="E234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>105</v>
-      </c>
-      <c r="E235" t="inlineStr"/>
+        <v>23</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -12152,282 +12510,282 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>13:31</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>13:38</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>52</v>
-      </c>
-      <c r="E237" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="E237" t="inlineStr"/>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>13:39</t>
+          <t>13:31</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="E238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>13:40</t>
+          <t>13:33</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>115</v>
-      </c>
-      <c r="E239" t="inlineStr"/>
+        <v>35</v>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>13:42</t>
+          <t>13:38</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>73</v>
-      </c>
-      <c r="E240" t="inlineStr"/>
+        <v>52</v>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>13:43</t>
+          <t>13:39</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>57</v>
-      </c>
-      <c r="E241" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:40</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>13:53</t>
+          <t>13:42</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="E243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:43</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>116</v>
-      </c>
-      <c r="E244" t="inlineStr"/>
+        <v>57</v>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:51</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="E245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:53</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="E246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="E247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>12:38:18</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>103</v>
-      </c>
-      <c r="E248" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -12437,37 +12795,37 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>14:24</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="E249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>14:25</t>
+          <t>14:11</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -12478,21 +12836,21 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -12503,46 +12861,42 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>14:37</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>116</v>
-      </c>
-      <c r="E252" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>14:40</t>
+          <t>14:20</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -12553,23 +12907,269 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
+          <t>12:38:18</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>103</v>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>12:29:23</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>14:24</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>115</v>
+      </c>
+      <c r="E255" t="inlineStr"/>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>14:25</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>104</v>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>95</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
           <t>12:46:01</t>
         </is>
       </c>
-      <c r="B254" t="inlineStr">
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>108</v>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>14:37</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>116</v>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>14:40</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D260" t="n">
+        <v>119</v>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>106</v>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>12:46:01</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
         <is>
           <t>14:45</t>
         </is>
       </c>
-      <c r="C254" t="inlineStr">
+      <c r="C262" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D254" t="n">
+      <c r="D262" t="n">
         <v>119</v>
       </c>
-      <c r="E254" t="inlineStr">
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D263" t="n">
+        <v>115</v>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>115</v>
+      </c>
+      <c r="E264" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 78
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E264"/>
+  <dimension ref="A1:E277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:58:39</t>
+          <t>Última actualización: 13:35:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 259</t>
+          <t>Total filas: 272</t>
         </is>
       </c>
     </row>
@@ -2944,7 +2944,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>07:51:22</t>
+          <t>08:22:12</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -2954,18 +2954,18 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="E123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>08:22:12</t>
+          <t>07:51:22</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -2975,11 +2975,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="E124" t="inlineStr"/>
     </row>
@@ -4036,7 +4036,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10:51:31</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4046,18 +4046,18 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>10:51:31</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4067,11 +4067,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E176" t="inlineStr"/>
     </row>
@@ -4372,7 +4372,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -4382,18 +4382,18 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="E191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -4403,11 +4403,11 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="E192" t="inlineStr"/>
     </row>
@@ -5287,7 +5287,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -5297,18 +5297,22 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>116</v>
-      </c>
-      <c r="E234" t="inlineStr"/>
+        <v>23</v>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -5318,17 +5322,13 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>23</v>
-      </c>
-      <c r="E235" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E235" t="inlineStr"/>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -5421,21 +5421,21 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>13:38</t>
+          <t>13:36</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -5446,12 +5446,12 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>13:39</t>
+          <t>13:38</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -5460,61 +5460,65 @@
         </is>
       </c>
       <c r="D241" t="n">
-        <v>70</v>
-      </c>
-      <c r="E241" t="inlineStr"/>
+        <v>52</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>13:40</t>
+          <t>13:39</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="E242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>13:42</t>
+          <t>13:40</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="E243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>13:43</t>
+          <t>13:42</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -5523,34 +5527,34 @@
         </is>
       </c>
       <c r="D244" t="n">
-        <v>57</v>
-      </c>
-      <c r="E244" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:43</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>113</v>
-      </c>
-      <c r="E245" t="inlineStr"/>
+        <v>57</v>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -5560,49 +5564,53 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>13:53</t>
+          <t>13:51</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:51</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>116</v>
-      </c>
-      <c r="E247" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:53</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -5611,74 +5619,70 @@
         </is>
       </c>
       <c r="D248" t="n">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="E248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="E249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>14:11</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>73</v>
-      </c>
-      <c r="E250" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -5694,37 +5698,37 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>14:03</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -5735,21 +5739,21 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>12:38:18</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:11</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -5760,42 +5764,46 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>14:24</t>
+          <t>14:14</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D255" t="n">
-        <v>115</v>
-      </c>
-      <c r="E255" t="inlineStr"/>
+        <v>39</v>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>14:25</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -5806,46 +5814,42 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>95</v>
-      </c>
-      <c r="E257" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:20</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -5856,21 +5860,21 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:38:18</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>14:37</t>
+          <t>14:21</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -5881,46 +5885,42 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>14:40</t>
+          <t>14:24</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>119</v>
-      </c>
-      <c r="E260" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:41:18</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>14:44</t>
+          <t>14:25</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -5931,21 +5931,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -5956,21 +5956,21 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -5981,23 +5981,348 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>59</v>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>14:37</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>116</v>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>14:38</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>63</v>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>14:40</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>119</v>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
           <t>12:58:39</t>
         </is>
       </c>
-      <c r="B264" t="inlineStr">
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D268" t="n">
+        <v>106</v>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>12:46:01</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D269" t="n">
+        <v>119</v>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
         <is>
           <t>14:53</t>
         </is>
       </c>
-      <c r="C264" t="inlineStr">
+      <c r="C270" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D264" t="n">
+      <c r="D270" t="n">
         <v>115</v>
       </c>
-      <c r="E264" t="inlineStr">
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>115</v>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>81</v>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>15:01</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>86</v>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>15:04</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>89</v>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>15:17</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>102</v>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>109</v>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>110</v>
+      </c>
+      <c r="E277" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6014,7 +6339,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6032,14 +6357,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:58:39</t>
+          <t>Última actualización: 13:35:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 71</t>
+          <t>Total filas: 73</t>
         </is>
       </c>
     </row>
@@ -6997,7 +7322,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -7007,18 +7332,18 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -7028,11 +7353,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E51" t="inlineStr"/>
     </row>
@@ -7584,6 +7909,56 @@
         <v>115</v>
       </c>
       <c r="E76" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>81</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>110</v>
+      </c>
+      <c r="E78" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7600,7 +7975,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E264"/>
+  <dimension ref="A1:E277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7618,14 +7993,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:58:39</t>
+          <t>Última actualización: 13:35:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 259</t>
+          <t>Total filas: 272</t>
         </is>
       </c>
     </row>
@@ -10116,7 +10491,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>07:51:22</t>
+          <t>08:22:12</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -10126,18 +10501,18 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="E123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>08:22:12</t>
+          <t>07:51:22</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -10147,11 +10522,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="E124" t="inlineStr"/>
     </row>
@@ -11208,7 +11583,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10:51:31</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -11218,18 +11593,18 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>10:51:31</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -11239,11 +11614,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E176" t="inlineStr"/>
     </row>
@@ -11544,7 +11919,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -11554,18 +11929,18 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="E191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -11575,11 +11950,11 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="E192" t="inlineStr"/>
     </row>
@@ -12459,7 +12834,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -12469,18 +12844,22 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>116</v>
-      </c>
-      <c r="E234" t="inlineStr"/>
+        <v>23</v>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -12490,17 +12869,13 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>23</v>
-      </c>
-      <c r="E235" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E235" t="inlineStr"/>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -12593,21 +12968,21 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>13:38</t>
+          <t>13:36</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -12618,12 +12993,12 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>13:39</t>
+          <t>13:38</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -12632,61 +13007,65 @@
         </is>
       </c>
       <c r="D241" t="n">
-        <v>70</v>
-      </c>
-      <c r="E241" t="inlineStr"/>
+        <v>52</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>13:40</t>
+          <t>13:39</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="E242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>13:42</t>
+          <t>13:40</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="E243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>13:43</t>
+          <t>13:42</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -12695,34 +13074,34 @@
         </is>
       </c>
       <c r="D244" t="n">
-        <v>57</v>
-      </c>
-      <c r="E244" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:43</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>113</v>
-      </c>
-      <c r="E245" t="inlineStr"/>
+        <v>57</v>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -12732,49 +13111,53 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>13:53</t>
+          <t>13:51</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:51</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>116</v>
-      </c>
-      <c r="E247" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:53</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -12783,74 +13166,70 @@
         </is>
       </c>
       <c r="D248" t="n">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="E248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="E249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>14:11</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>73</v>
-      </c>
-      <c r="E250" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -12866,37 +13245,37 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>14:03</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -12907,21 +13286,21 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>12:38:18</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:11</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -12932,42 +13311,46 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>14:24</t>
+          <t>14:14</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D255" t="n">
-        <v>115</v>
-      </c>
-      <c r="E255" t="inlineStr"/>
+        <v>39</v>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>14:25</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -12978,46 +13361,42 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>95</v>
-      </c>
-      <c r="E257" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:20</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -13028,21 +13407,21 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:38:18</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>14:37</t>
+          <t>14:21</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -13053,46 +13432,42 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>14:40</t>
+          <t>14:24</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>119</v>
-      </c>
-      <c r="E260" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:41:18</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>14:44</t>
+          <t>14:25</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -13103,21 +13478,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -13128,21 +13503,21 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -13153,23 +13528,348 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>59</v>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>14:37</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>116</v>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>14:38</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>63</v>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>12:41:18</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>14:40</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>119</v>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
           <t>12:58:39</t>
         </is>
       </c>
-      <c r="B264" t="inlineStr">
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D268" t="n">
+        <v>106</v>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>12:46:01</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D269" t="n">
+        <v>119</v>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
         <is>
           <t>14:53</t>
         </is>
       </c>
-      <c r="C264" t="inlineStr">
+      <c r="C270" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D264" t="n">
+      <c r="D270" t="n">
         <v>115</v>
       </c>
-      <c r="E264" t="inlineStr">
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>12:58:39</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>115</v>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>81</v>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>15:01</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>86</v>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>15:04</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>89</v>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>15:17</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>102</v>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>109</v>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>110</v>
+      </c>
+      <c r="E277" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 79
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E277"/>
+  <dimension ref="A1:E286"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:35:25</t>
+          <t>Última actualización: 13:54:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 272</t>
+          <t>Total filas: 281</t>
         </is>
       </c>
     </row>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -3437,7 +3437,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D146" t="n">
@@ -3458,7 +3458,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D147" t="n">
@@ -4183,7 +4183,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4193,18 +4193,18 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -4214,11 +4214,11 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E183" t="inlineStr"/>
     </row>
@@ -4372,7 +4372,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -4382,18 +4382,18 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="E191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -4403,11 +4403,11 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="E192" t="inlineStr"/>
     </row>
@@ -4561,7 +4561,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>10:51:31</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -4571,18 +4571,18 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="E200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>10:51:31</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -4592,11 +4592,11 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="E201" t="inlineStr"/>
     </row>
@@ -4901,7 +4901,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -4911,13 +4911,17 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>76</v>
-      </c>
-      <c r="E216" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -4943,7 +4947,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -4953,17 +4957,13 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>3</v>
-      </c>
-      <c r="E218" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -5287,7 +5287,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -5297,22 +5297,18 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>23</v>
-      </c>
-      <c r="E234" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -5322,13 +5318,17 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>116</v>
-      </c>
-      <c r="E235" t="inlineStr"/>
+        <v>23</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -5668,21 +5668,21 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:55</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -5719,16 +5719,16 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>14:03</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -5739,21 +5739,21 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>14:11</t>
+          <t>14:03</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -5764,21 +5764,21 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>14:14</t>
+          <t>14:05</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D255" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -5794,16 +5794,16 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:11</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -5814,42 +5814,46 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:13</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>108</v>
-      </c>
-      <c r="E257" t="inlineStr"/>
+        <v>19</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>14:14</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -5860,21 +5864,21 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>12:38:18</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -5890,37 +5894,37 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>14:24</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>14:25</t>
+          <t>14:20</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -5931,21 +5935,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:38:18</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>14:21</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -5956,46 +5960,42 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:24</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>108</v>
-      </c>
-      <c r="E263" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:41:18</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:25</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6006,21 +6006,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>14:37</t>
+          <t>14:31</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6031,21 +6031,21 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>14:38</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -6056,21 +6056,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>14:40</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>119</v>
+        <v>59</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -6081,21 +6081,21 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>14:44</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -6106,21 +6106,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:41:18</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:37</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -6131,21 +6131,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:38</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -6156,21 +6156,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:41:18</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:40</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -6181,21 +6181,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:44</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -6206,21 +6206,21 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>15:01</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -6231,12 +6231,12 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -6245,7 +6245,7 @@
         </is>
       </c>
       <c r="D274" t="n">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -6256,21 +6256,21 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -6286,16 +6286,16 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>14:56</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -6311,18 +6311,243 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
+          <t>15:01</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>86</v>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>15:02</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>68</v>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>15:04</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>89</v>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>71</v>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>15:17</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>102</v>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>109</v>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
           <t>15:25</t>
         </is>
       </c>
-      <c r="C277" t="inlineStr">
+      <c r="C283" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D277" t="n">
+      <c r="D283" t="n">
         <v>110</v>
       </c>
-      <c r="E277" t="inlineStr">
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>91</v>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>91</v>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>15:36</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>102</v>
+      </c>
+      <c r="E286" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6339,7 +6564,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6357,14 +6582,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:35:25</t>
+          <t>Última actualización: 13:54:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 73</t>
+          <t>Total filas: 74</t>
         </is>
       </c>
     </row>
@@ -7322,7 +7547,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -7332,18 +7557,18 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -7353,11 +7578,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E51" t="inlineStr"/>
     </row>
@@ -7942,23 +8167,48 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>15:02</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>68</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
           <t>13:35:25</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
+      <c r="B79" t="inlineStr">
         <is>
           <t>15:25</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="C79" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D78" t="n">
+      <c r="D79" t="n">
         <v>110</v>
       </c>
-      <c r="E78" t="inlineStr">
+      <c r="E79" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7975,7 +8225,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E277"/>
+  <dimension ref="A1:E286"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7993,14 +8243,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:35:25</t>
+          <t>Última actualización: 13:54:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 272</t>
+          <t>Total filas: 281</t>
         </is>
       </c>
     </row>
@@ -9325,7 +9575,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -9346,7 +9596,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -10984,7 +11234,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D146" t="n">
@@ -11005,7 +11255,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D147" t="n">
@@ -11730,7 +11980,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -11740,18 +11990,18 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -11761,11 +12011,11 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E183" t="inlineStr"/>
     </row>
@@ -11919,7 +12169,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -11929,18 +12179,18 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="E191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -11950,11 +12200,11 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="E192" t="inlineStr"/>
     </row>
@@ -12108,7 +12358,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>10:51:31</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -12118,18 +12368,18 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="E200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>10:51:31</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -12139,11 +12389,11 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="E201" t="inlineStr"/>
     </row>
@@ -12448,7 +12698,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -12458,13 +12708,17 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>76</v>
-      </c>
-      <c r="E216" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -12490,7 +12744,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -12500,17 +12754,13 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>3</v>
-      </c>
-      <c r="E218" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -12834,7 +13084,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -12844,22 +13094,18 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>23</v>
-      </c>
-      <c r="E234" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -12869,13 +13115,17 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>116</v>
-      </c>
-      <c r="E235" t="inlineStr"/>
+        <v>23</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -13215,21 +13465,21 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:55</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -13266,16 +13516,16 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>14:03</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -13286,21 +13536,21 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>14:11</t>
+          <t>14:03</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -13311,21 +13561,21 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>14:14</t>
+          <t>14:05</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D255" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -13341,16 +13591,16 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:11</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -13361,42 +13611,46 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:13</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>108</v>
-      </c>
-      <c r="E257" t="inlineStr"/>
+        <v>19</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>14:14</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -13407,21 +13661,21 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>12:38:18</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -13437,37 +13691,37 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>14:24</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>14:25</t>
+          <t>14:20</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -13478,21 +13732,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:38:18</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>14:21</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -13503,46 +13757,42 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:24</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>108</v>
-      </c>
-      <c r="E263" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:41:18</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:25</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -13553,21 +13803,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>14:37</t>
+          <t>14:31</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -13578,21 +13828,21 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>14:38</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -13603,21 +13853,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>14:40</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>119</v>
+        <v>59</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -13628,21 +13878,21 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>14:44</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -13653,21 +13903,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:41:18</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:37</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -13678,21 +13928,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:38</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -13703,21 +13953,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:41:18</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:40</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -13728,21 +13978,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:44</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -13753,21 +14003,21 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>15:01</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -13778,12 +14028,12 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -13792,7 +14042,7 @@
         </is>
       </c>
       <c r="D274" t="n">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -13803,21 +14053,21 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -13833,16 +14083,16 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>14:56</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -13858,18 +14108,243 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
+          <t>15:01</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>86</v>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>15:02</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>68</v>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>15:04</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>89</v>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>71</v>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>15:17</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>102</v>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>109</v>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
           <t>15:25</t>
         </is>
       </c>
-      <c r="C277" t="inlineStr">
+      <c r="C283" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D277" t="n">
+      <c r="D283" t="n">
         <v>110</v>
       </c>
-      <c r="E277" t="inlineStr">
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>91</v>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>91</v>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>15:36</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>102</v>
+      </c>
+      <c r="E286" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 80
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E286"/>
+  <dimension ref="A1:E296"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:54:15</t>
+          <t>Última actualización: 14:23:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 281</t>
+          <t>Total filas: 291</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -665,18 +665,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -686,11 +686,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -2786,7 +2786,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -2944,7 +2944,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>08:22:12</t>
+          <t>07:51:22</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -2954,18 +2954,18 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="E123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>07:51:22</t>
+          <t>08:22:12</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -2975,11 +2975,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="E124" t="inlineStr"/>
     </row>
@@ -3532,7 +3532,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>08:41:14</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -3542,18 +3542,18 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>113</v>
+        <v>37</v>
       </c>
       <c r="E151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>08:41:14</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="E152" t="inlineStr"/>
     </row>
@@ -6031,7 +6031,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -6041,11 +6041,11 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -6056,21 +6056,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -6081,7 +6081,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -6091,11 +6091,11 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -6106,21 +6106,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>14:37</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -6131,21 +6131,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:41:18</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>14:38</t>
+          <t>14:37</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -6156,21 +6156,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>14:40</t>
+          <t>14:38</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>119</v>
+        <v>63</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -6181,21 +6181,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:41:18</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>14:44</t>
+          <t>14:40</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -6206,12 +6206,12 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:44</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -6220,7 +6220,7 @@
         </is>
       </c>
       <c r="D273" t="n">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -6231,21 +6231,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -6256,21 +6256,21 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:49</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>115</v>
+        <v>26</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -6281,21 +6281,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -6306,21 +6306,21 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>15:01</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -6331,12 +6331,12 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>14:56</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -6345,7 +6345,7 @@
         </is>
       </c>
       <c r="D278" t="n">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -6361,16 +6361,16 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>15:01</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -6386,16 +6386,16 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -6406,21 +6406,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:03</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>102</v>
+        <v>40</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -6436,16 +6436,16 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -6456,21 +6456,21 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>110</v>
+        <v>41</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -6486,16 +6486,16 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -6506,12 +6506,12 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -6520,7 +6520,7 @@
         </is>
       </c>
       <c r="D285" t="n">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -6531,23 +6531,273 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>109</v>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D287" t="n">
+        <v>61</v>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>110</v>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
           <t>13:54:15</t>
         </is>
       </c>
-      <c r="B286" t="inlineStr">
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>91</v>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D290" t="n">
+        <v>91</v>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
         <is>
           <t>15:36</t>
         </is>
       </c>
-      <c r="C286" t="inlineStr">
+      <c r="C291" t="inlineStr">
         <is>
           <t>17X38_ROMERO</t>
         </is>
       </c>
-      <c r="D286" t="n">
+      <c r="D291" t="n">
         <v>102</v>
       </c>
-      <c r="E286" t="inlineStr">
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>15:44</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>81</v>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D293" t="n">
+        <v>82</v>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>15:55</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>92</v>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>98</v>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>117</v>
+      </c>
+      <c r="E296" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6564,7 +6814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6582,14 +6832,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:54:15</t>
+          <t>Última actualización: 14:23:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 74</t>
+          <t>Total filas: 76</t>
         </is>
       </c>
     </row>
@@ -7589,7 +7839,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -7599,18 +7849,18 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="E52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -7620,11 +7870,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="E53" t="inlineStr"/>
     </row>
@@ -8192,23 +8442,73 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>61</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
           <t>13:35:25</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="B80" t="inlineStr">
         <is>
           <t>15:25</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D79" t="n">
+      <c r="D80" t="n">
         <v>110</v>
       </c>
-      <c r="E79" t="inlineStr">
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>82</v>
+      </c>
+      <c r="E81" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8225,7 +8525,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E286"/>
+  <dimension ref="A1:E296"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8243,14 +8543,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:54:15</t>
+          <t>Última actualización: 14:23:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 281</t>
+          <t>Total filas: 291</t>
         </is>
       </c>
     </row>
@@ -8452,7 +8752,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -8462,18 +8762,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -8483,11 +8783,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -9575,7 +9875,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -9596,7 +9896,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -10562,7 +10862,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -10583,7 +10883,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -10741,7 +11041,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>08:22:12</t>
+          <t>07:51:22</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -10751,18 +11051,18 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="E123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>07:51:22</t>
+          <t>08:22:12</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -10772,11 +11072,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="E124" t="inlineStr"/>
     </row>
@@ -11329,7 +11629,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>08:41:14</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -11339,18 +11639,18 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>113</v>
+        <v>37</v>
       </c>
       <c r="E151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>08:41:14</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -11360,11 +11660,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="E152" t="inlineStr"/>
     </row>
@@ -13828,7 +14128,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -13838,11 +14138,11 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -13853,21 +14153,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -13878,7 +14178,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -13888,11 +14188,11 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -13903,21 +14203,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>14:37</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -13928,21 +14228,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:41:18</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>14:38</t>
+          <t>14:37</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -13953,21 +14253,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>12:41:18</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>14:40</t>
+          <t>14:38</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>119</v>
+        <v>63</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -13978,21 +14278,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:41:18</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>14:44</t>
+          <t>14:40</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -14003,12 +14303,12 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:44</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -14017,7 +14317,7 @@
         </is>
       </c>
       <c r="D273" t="n">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -14028,21 +14328,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -14053,21 +14353,21 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:49</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>115</v>
+        <v>26</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -14078,21 +14378,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -14103,21 +14403,21 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>15:01</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -14128,12 +14428,12 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>14:56</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -14142,7 +14442,7 @@
         </is>
       </c>
       <c r="D278" t="n">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -14158,16 +14458,16 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>15:01</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -14183,16 +14483,16 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -14203,21 +14503,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:03</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>102</v>
+        <v>40</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -14233,16 +14533,16 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -14253,21 +14553,21 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>110</v>
+        <v>41</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -14283,16 +14583,16 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -14303,12 +14603,12 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -14317,7 +14617,7 @@
         </is>
       </c>
       <c r="D285" t="n">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -14328,23 +14628,273 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>109</v>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D287" t="n">
+        <v>61</v>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>110</v>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
           <t>13:54:15</t>
         </is>
       </c>
-      <c r="B286" t="inlineStr">
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>91</v>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D290" t="n">
+        <v>91</v>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
         <is>
           <t>15:36</t>
         </is>
       </c>
-      <c r="C286" t="inlineStr">
+      <c r="C291" t="inlineStr">
         <is>
           <t>17X38_ROMERO</t>
         </is>
       </c>
-      <c r="D286" t="n">
+      <c r="D291" t="n">
         <v>102</v>
       </c>
-      <c r="E286" t="inlineStr">
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>15:44</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>81</v>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D293" t="n">
+        <v>82</v>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>15:55</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>92</v>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>98</v>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>117</v>
+      </c>
+      <c r="E296" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 81
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E296"/>
+  <dimension ref="A1:E309"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:23:38</t>
+          <t>Última actualización: 14:43:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 291</t>
+          <t>Total filas: 304</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -665,18 +665,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -686,11 +686,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -2041,7 +2041,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>07:31:04</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2051,18 +2051,18 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="E80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>07:31:04</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2072,11 +2072,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="E81" t="inlineStr"/>
     </row>
@@ -2629,7 +2629,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>07:31:04</t>
+          <t>07:51:22</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2639,18 +2639,18 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="E108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>07:51:22</t>
+          <t>07:31:04</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2660,11 +2660,11 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="E109" t="inlineStr"/>
     </row>
@@ -4036,7 +4036,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>10:51:31</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4046,18 +4046,18 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>10:51:31</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4067,11 +4067,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E176" t="inlineStr"/>
     </row>
@@ -4225,7 +4225,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4235,18 +4235,18 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="E184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4256,18 +4256,18 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="E185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4277,11 +4277,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E186" t="inlineStr"/>
     </row>
@@ -4466,7 +4466,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D195" t="n">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -5035,7 +5035,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -5045,18 +5045,18 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="E222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5066,11 +5066,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E223" t="inlineStr"/>
     </row>
@@ -5693,7 +5693,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -5703,18 +5703,22 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>92</v>
-      </c>
-      <c r="E252" t="inlineStr"/>
+        <v>26</v>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -5724,17 +5728,13 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>26</v>
-      </c>
-      <c r="E253" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -6281,21 +6281,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:51</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>115</v>
+        <v>8</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -6331,21 +6331,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -6356,21 +6356,21 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>15:01</t>
+          <t>14:54</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -6381,12 +6381,12 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>14:56</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -6395,7 +6395,7 @@
         </is>
       </c>
       <c r="D280" t="n">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -6406,21 +6406,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>15:03</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -6436,16 +6436,16 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>15:01</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -6456,21 +6456,21 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -6481,21 +6481,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>15:03</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -6511,16 +6511,16 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -6531,21 +6531,21 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -6556,21 +6556,21 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -6581,21 +6581,21 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>110</v>
+        <v>71</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -6606,21 +6606,21 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -6631,21 +6631,21 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:24</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -6656,21 +6656,21 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>15:24</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -6681,21 +6681,21 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>15:25</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -6706,21 +6706,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:25</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -6731,21 +6731,21 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>15:25</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -6756,21 +6756,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>15:36</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -6786,18 +6786,343 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
+          <t>15:44</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>81</v>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>82</v>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>70</v>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>15:55</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D299" t="n">
+        <v>92</v>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>73</v>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>98</v>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
           <t>16:20</t>
         </is>
       </c>
-      <c r="C296" t="inlineStr">
+      <c r="C302" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D296" t="n">
+      <c r="D302" t="n">
         <v>117</v>
       </c>
-      <c r="E296" t="inlineStr">
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D303" t="n">
+        <v>101</v>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>101</v>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>16:25</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D305" t="n">
+        <v>102</v>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>16:31</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>108</v>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D307" t="n">
+        <v>110</v>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>111</v>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>16:36</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>113</v>
+      </c>
+      <c r="E309" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6814,7 +7139,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6832,14 +7157,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:23:38</t>
+          <t>Última actualización: 14:43:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 76</t>
+          <t>Total filas: 80</t>
         </is>
       </c>
     </row>
@@ -8442,21 +8767,21 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -8467,12 +8792,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:24</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -8481,7 +8806,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -8492,23 +8817,123 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
+          <t>13:35:25</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>110</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
           <t>14:23:38</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="B82" t="inlineStr">
         <is>
           <t>15:45</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="C82" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D81" t="n">
+      <c r="D82" t="n">
         <v>82</v>
       </c>
-      <c r="E81" t="inlineStr">
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>70</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>101</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>16:25</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>102</v>
+      </c>
+      <c r="E85" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8525,7 +8950,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E296"/>
+  <dimension ref="A1:E309"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8543,14 +8968,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:23:38</t>
+          <t>Última actualización: 14:43:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 291</t>
+          <t>Total filas: 304</t>
         </is>
       </c>
     </row>
@@ -8752,7 +9177,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -8762,18 +9187,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -8783,11 +9208,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -10138,7 +10563,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>07:31:04</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -10148,18 +10573,18 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="E80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>07:31:04</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -10169,11 +10594,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="E81" t="inlineStr"/>
     </row>
@@ -10726,7 +11151,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>07:31:04</t>
+          <t>07:51:22</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -10736,18 +11161,18 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="E108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>07:51:22</t>
+          <t>07:31:04</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -10757,11 +11182,11 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="E109" t="inlineStr"/>
     </row>
@@ -12133,7 +12558,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>10:51:31</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -12143,18 +12568,18 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>10:51:31</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -12164,11 +12589,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E176" t="inlineStr"/>
     </row>
@@ -12322,7 +12747,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -12332,18 +12757,18 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="E184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -12353,18 +12778,18 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="E185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -12374,11 +12799,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E186" t="inlineStr"/>
     </row>
@@ -12563,7 +12988,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D195" t="n">
@@ -12584,7 +13009,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -13132,7 +13557,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -13142,18 +13567,18 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="E222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -13163,11 +13588,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E223" t="inlineStr"/>
     </row>
@@ -13790,7 +14215,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -13800,18 +14225,22 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>92</v>
-      </c>
-      <c r="E252" t="inlineStr"/>
+        <v>26</v>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -13821,17 +14250,13 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>26</v>
-      </c>
-      <c r="E253" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -14378,21 +14803,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:51</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>115</v>
+        <v>8</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -14428,21 +14853,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -14453,21 +14878,21 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>15:01</t>
+          <t>14:54</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -14478,12 +14903,12 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>14:56</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -14492,7 +14917,7 @@
         </is>
       </c>
       <c r="D280" t="n">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -14503,21 +14928,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>15:03</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -14533,16 +14958,16 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>15:01</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -14553,21 +14978,21 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -14578,21 +15003,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>15:03</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -14608,16 +15033,16 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -14628,21 +15053,21 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -14653,21 +15078,21 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -14678,21 +15103,21 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>110</v>
+        <v>71</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -14703,21 +15128,21 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -14728,21 +15153,21 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:24</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -14753,21 +15178,21 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>15:24</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -14778,21 +15203,21 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>15:25</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -14803,21 +15228,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:25</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -14828,21 +15253,21 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>15:25</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -14853,21 +15278,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>15:36</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -14883,18 +15308,343 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
+          <t>15:44</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>81</v>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>82</v>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>70</v>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>15:55</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D299" t="n">
+        <v>92</v>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>73</v>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>98</v>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>14:23:38</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
           <t>16:20</t>
         </is>
       </c>
-      <c r="C296" t="inlineStr">
+      <c r="C302" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D296" t="n">
+      <c r="D302" t="n">
         <v>117</v>
       </c>
-      <c r="E296" t="inlineStr">
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D303" t="n">
+        <v>101</v>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>101</v>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>16:25</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D305" t="n">
+        <v>102</v>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>16:31</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>108</v>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D307" t="n">
+        <v>110</v>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>111</v>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>16:36</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>113</v>
+      </c>
+      <c r="E309" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 82
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E309"/>
+  <dimension ref="A1:E319"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:43:48</t>
+          <t>Última actualización: 14:57:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 304</t>
+          <t>Total filas: 314</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -665,18 +665,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -686,11 +686,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1295,7 +1295,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -2041,7 +2041,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>07:31:04</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2051,18 +2051,18 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="E80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>07:31:04</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2072,11 +2072,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="E81" t="inlineStr"/>
     </row>
@@ -3532,7 +3532,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>08:41:14</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -3542,18 +3542,18 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="E151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>08:41:14</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>113</v>
+        <v>37</v>
       </c>
       <c r="E152" t="inlineStr"/>
     </row>
@@ -4561,7 +4561,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>10:51:31</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -4571,18 +4571,18 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="E200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>10:51:31</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -4592,11 +4592,11 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="E201" t="inlineStr"/>
     </row>
@@ -5161,7 +5161,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -5171,18 +5171,18 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="E228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -5192,11 +5192,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="E229" t="inlineStr"/>
     </row>
@@ -5343,7 +5343,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -5364,7 +5364,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -5626,7 +5626,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -5636,18 +5636,18 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="E249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -5657,11 +5657,11 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="E250" t="inlineStr"/>
     </row>
@@ -6406,21 +6406,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:58</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -6431,21 +6431,21 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>15:01</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -6456,21 +6456,21 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>15:01</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -6481,21 +6481,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>15:03</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -6506,21 +6506,21 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>89</v>
+        <v>5</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -6536,16 +6536,16 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>15:03</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -6556,7 +6556,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -6566,11 +6566,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -6581,21 +6581,21 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -6606,21 +6606,21 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -6631,21 +6631,21 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -6656,21 +6656,21 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -6681,21 +6681,21 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:24</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -6706,12 +6706,12 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:24</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -6720,7 +6720,7 @@
         </is>
       </c>
       <c r="D293" t="n">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -6731,7 +6731,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -6741,11 +6741,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -6761,16 +6761,16 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>15:25</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -6781,21 +6781,21 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>15:25</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -6806,21 +6806,21 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:33</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -6831,21 +6831,21 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:36</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -6861,16 +6861,16 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>15:44</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -6881,21 +6881,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -6906,21 +6906,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>15:51</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -6931,21 +6931,21 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -6956,21 +6956,21 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>15:55</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -6986,16 +6986,16 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7006,21 +7006,21 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>16:25</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7031,21 +7031,21 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>16:31</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -7056,21 +7056,21 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -7081,21 +7081,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:22</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -7111,18 +7111,268 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>101</v>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>101</v>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>16:25</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>102</v>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>16:31</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>108</v>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>110</v>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>96</v>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>111</v>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
           <t>16:36</t>
         </is>
       </c>
-      <c r="C309" t="inlineStr">
+      <c r="C316" t="inlineStr">
         <is>
           <t>17X38_ROMERO</t>
         </is>
       </c>
-      <c r="D309" t="n">
+      <c r="D316" t="n">
         <v>113</v>
       </c>
-      <c r="E309" t="inlineStr">
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D317" t="n">
+        <v>104</v>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>116</v>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>119</v>
+      </c>
+      <c r="E319" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7139,7 +7389,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7157,14 +7407,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:43:48</t>
+          <t>Última actualización: 14:57:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 80</t>
+          <t>Total filas: 82</t>
         </is>
       </c>
     </row>
@@ -8867,12 +9117,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:51</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -8881,7 +9131,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -8897,16 +9147,16 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -8922,18 +9172,68 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>101</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
           <t>16:25</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr">
+      <c r="C86" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D85" t="n">
+      <c r="D86" t="n">
         <v>102</v>
       </c>
-      <c r="E85" t="inlineStr">
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>119</v>
+      </c>
+      <c r="E87" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8950,7 +9250,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E309"/>
+  <dimension ref="A1:E319"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8968,14 +9268,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:43:48</t>
+          <t>Última actualización: 14:57:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 304</t>
+          <t>Total filas: 314</t>
         </is>
       </c>
     </row>
@@ -9177,7 +9477,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -9187,18 +9487,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -9208,11 +9508,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -9796,7 +10096,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -9817,7 +10117,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -10563,7 +10863,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>07:31:04</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -10573,18 +10873,18 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="E80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>07:31:04</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -10594,11 +10894,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="E81" t="inlineStr"/>
     </row>
@@ -12054,7 +12354,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>08:41:14</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -12064,18 +12364,18 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="E151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>08:41:14</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -12085,11 +12385,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>113</v>
+        <v>37</v>
       </c>
       <c r="E152" t="inlineStr"/>
     </row>
@@ -13083,7 +13383,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>10:51:31</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -13093,18 +13393,18 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="E200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>10:51:31</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -13114,11 +13414,11 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="E201" t="inlineStr"/>
     </row>
@@ -13683,7 +13983,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -13693,18 +13993,18 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="E228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -13714,11 +14014,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="E229" t="inlineStr"/>
     </row>
@@ -13865,7 +14165,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -13886,7 +14186,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -14148,7 +14448,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -14158,18 +14458,18 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="E249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -14179,11 +14479,11 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="E250" t="inlineStr"/>
     </row>
@@ -14928,21 +15228,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:58</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -14953,21 +15253,21 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>15:01</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -14978,21 +15278,21 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>15:01</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -15003,21 +15303,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>15:03</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -15028,21 +15328,21 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>89</v>
+        <v>5</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -15058,16 +15358,16 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>15:03</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -15078,7 +15378,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -15088,11 +15388,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -15103,21 +15403,21 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -15128,21 +15428,21 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -15153,21 +15453,21 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -15178,21 +15478,21 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -15203,21 +15503,21 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:24</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -15228,12 +15528,12 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:24</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -15242,7 +15542,7 @@
         </is>
       </c>
       <c r="D293" t="n">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -15253,7 +15553,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -15263,11 +15563,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -15283,16 +15583,16 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>15:25</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -15303,21 +15603,21 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>15:25</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -15328,21 +15628,21 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:33</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -15353,21 +15653,21 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:36</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -15383,16 +15683,16 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>15:44</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -15403,21 +15703,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -15428,21 +15728,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>15:51</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -15453,21 +15753,21 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -15478,21 +15778,21 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>15:55</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -15508,16 +15808,16 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -15528,21 +15828,21 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>16:25</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -15553,21 +15853,21 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>16:31</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -15578,21 +15878,21 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -15603,21 +15903,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:22</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -15633,18 +15933,268 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>101</v>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>101</v>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>16:25</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>102</v>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>16:31</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>108</v>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>110</v>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>96</v>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>111</v>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
           <t>16:36</t>
         </is>
       </c>
-      <c r="C309" t="inlineStr">
+      <c r="C316" t="inlineStr">
         <is>
           <t>17X38_ROMERO</t>
         </is>
       </c>
-      <c r="D309" t="n">
+      <c r="D316" t="n">
         <v>113</v>
       </c>
-      <c r="E309" t="inlineStr">
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D317" t="n">
+        <v>104</v>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>116</v>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>119</v>
+      </c>
+      <c r="E319" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 83
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E319"/>
+  <dimension ref="A1:E337"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:57:55</t>
+          <t>Última actualización: 15:40:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 314</t>
+          <t>Total filas: 332</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -665,18 +665,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -686,11 +686,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1337,7 +1337,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1726,7 +1726,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1736,18 +1736,18 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="E65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>06:45:29</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1757,11 +1757,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="E66" t="inlineStr"/>
     </row>
@@ -1915,7 +1915,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1925,18 +1925,18 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="E74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1946,11 +1946,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E75" t="inlineStr"/>
     </row>
@@ -2146,7 +2146,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>06:58:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2156,18 +2156,18 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="E85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2177,11 +2177,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E86" t="inlineStr"/>
     </row>
@@ -2629,7 +2629,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>07:51:22</t>
+          <t>07:31:04</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2639,18 +2639,18 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="E108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>07:31:04</t>
+          <t>07:51:22</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2660,11 +2660,11 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="E109" t="inlineStr"/>
     </row>
@@ -3280,7 +3280,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>08:57:53</t>
+          <t>08:22:12</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -3290,18 +3290,18 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="E139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>08:22:12</t>
+          <t>08:57:53</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3311,11 +3311,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="E140" t="inlineStr"/>
     </row>
@@ -4372,7 +4372,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -4382,18 +4382,18 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="E191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -4403,11 +4403,11 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="E192" t="inlineStr"/>
     </row>
@@ -5035,7 +5035,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -5045,18 +5045,18 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5066,11 +5066,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="E223" t="inlineStr"/>
     </row>
@@ -6481,7 +6481,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -6491,11 +6491,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -6506,7 +6506,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -6516,11 +6516,11 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -6731,7 +6731,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -6741,11 +6741,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -6766,7 +6766,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -6781,7 +6781,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -6791,11 +6791,11 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -6906,12 +6906,12 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>15:51</t>
+          <t>15:48</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -6920,7 +6920,7 @@
         </is>
       </c>
       <c r="D301" t="n">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -6931,12 +6931,12 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:51</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -6945,7 +6945,7 @@
         </is>
       </c>
       <c r="D302" t="n">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -6956,21 +6956,21 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -6981,12 +6981,12 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:55</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -6995,7 +6995,7 @@
         </is>
       </c>
       <c r="D304" t="n">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7006,21 +7006,21 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7031,21 +7031,21 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>16:16</t>
+          <t>15:57</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -7061,16 +7061,16 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -7081,21 +7081,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>16:22</t>
+          <t>16:03</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -7106,21 +7106,21 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -7131,21 +7131,21 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -7156,21 +7156,21 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>16:25</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -7181,21 +7181,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>16:31</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -7206,21 +7206,21 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:22</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -7231,21 +7231,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:24</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -7261,16 +7261,16 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:24</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -7281,21 +7281,21 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:25</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -7306,21 +7306,21 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:25</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -7331,21 +7331,21 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:26</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D318" t="n">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -7356,23 +7356,473 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>16:31</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>108</v>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>16:32</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>52</v>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>110</v>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
           <t>14:57:55</t>
         </is>
       </c>
-      <c r="B319" t="inlineStr">
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>96</v>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>111</v>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>16:36</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>113</v>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>16:38</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>58</v>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D326" t="n">
+        <v>104</v>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>116</v>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
         <is>
           <t>16:56</t>
         </is>
       </c>
-      <c r="C319" t="inlineStr">
+      <c r="C328" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D319" t="n">
+      <c r="D328" t="n">
         <v>119</v>
       </c>
-      <c r="E319" t="inlineStr">
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D329" t="n">
+        <v>77</v>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D330" t="n">
+        <v>77</v>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>17:03</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D331" t="n">
+        <v>83</v>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>17:17</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>97</v>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
+        <v>104</v>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>114</v>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>115</v>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D336" t="n">
+        <v>116</v>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>118</v>
+      </c>
+      <c r="E337" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7389,7 +7839,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7407,14 +7857,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:57:55</t>
+          <t>Última actualización: 15:40:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 82</t>
+          <t>Total filas: 87</t>
         </is>
       </c>
     </row>
@@ -7899,7 +8349,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -7920,7 +8370,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -9117,12 +9567,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>15:51</t>
+          <t>15:48</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -9131,7 +9581,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -9142,12 +9592,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:51</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -9156,7 +9606,7 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -9172,16 +9622,16 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -9197,16 +9647,16 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>16:25</t>
+          <t>16:24</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -9217,23 +9667,148 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>16:25</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>102</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>16:25</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>45</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>16:26</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>46</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
           <t>14:57:55</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B90" t="inlineStr">
         <is>
           <t>16:56</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="C90" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D87" t="n">
+      <c r="D90" t="n">
         <v>119</v>
       </c>
-      <c r="E87" t="inlineStr">
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>77</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>77</v>
+      </c>
+      <c r="E92" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9250,7 +9825,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E319"/>
+  <dimension ref="A1:E337"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9268,14 +9843,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:57:55</t>
+          <t>Última actualización: 15:40:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 314</t>
+          <t>Total filas: 332</t>
         </is>
       </c>
     </row>
@@ -9477,7 +10052,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -9487,18 +10062,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -9508,11 +10083,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -10138,7 +10713,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -10159,7 +10734,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -10548,7 +11123,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:45:29</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -10558,18 +11133,18 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="E65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>06:45:29</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -10579,11 +11154,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="E66" t="inlineStr"/>
     </row>
@@ -10737,7 +11312,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>05:55:51</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -10747,18 +11322,18 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="E74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>05:55:51</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -10768,11 +11343,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E75" t="inlineStr"/>
     </row>
@@ -10968,7 +11543,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>06:58:06</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -10978,18 +11553,18 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="E85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -10999,11 +11574,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E86" t="inlineStr"/>
     </row>
@@ -11451,7 +12026,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>07:51:22</t>
+          <t>07:31:04</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -11461,18 +12036,18 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="E108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>07:31:04</t>
+          <t>07:51:22</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -11482,11 +12057,11 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="E109" t="inlineStr"/>
     </row>
@@ -12102,7 +12677,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>08:57:53</t>
+          <t>08:22:12</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -12112,18 +12687,18 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="E139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>08:22:12</t>
+          <t>08:57:53</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -12133,11 +12708,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="E140" t="inlineStr"/>
     </row>
@@ -13194,7 +13769,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -13204,18 +13779,18 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="E191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -13225,11 +13800,11 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="E192" t="inlineStr"/>
     </row>
@@ -13857,7 +14432,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -13867,18 +14442,18 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -13888,11 +14463,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="E223" t="inlineStr"/>
     </row>
@@ -15303,7 +15878,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -15313,11 +15888,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -15328,7 +15903,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -15338,11 +15913,11 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -15553,7 +16128,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -15563,11 +16138,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -15588,7 +16163,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -15603,7 +16178,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -15613,11 +16188,11 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -15728,12 +16303,12 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>15:51</t>
+          <t>15:48</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -15742,7 +16317,7 @@
         </is>
       </c>
       <c r="D301" t="n">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -15753,12 +16328,12 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:51</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -15767,7 +16342,7 @@
         </is>
       </c>
       <c r="D302" t="n">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -15778,21 +16353,21 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -15803,12 +16378,12 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:55</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -15817,7 +16392,7 @@
         </is>
       </c>
       <c r="D304" t="n">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -15828,21 +16403,21 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -15853,21 +16428,21 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>16:16</t>
+          <t>15:57</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -15883,16 +16458,16 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -15903,21 +16478,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>16:22</t>
+          <t>16:03</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -15928,21 +16503,21 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -15953,21 +16528,21 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -15978,21 +16553,21 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>16:25</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -16003,21 +16578,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>16:31</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -16028,21 +16603,21 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:22</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -16053,21 +16628,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:24</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -16083,16 +16658,16 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:24</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -16103,21 +16678,21 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:25</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -16128,21 +16703,21 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:25</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -16153,21 +16728,21 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:26</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D318" t="n">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -16178,23 +16753,473 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>16:31</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>108</v>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>16:32</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>52</v>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>110</v>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
           <t>14:57:55</t>
         </is>
       </c>
-      <c r="B319" t="inlineStr">
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>96</v>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>111</v>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>14:43:48</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>16:36</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>113</v>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>16:38</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>58</v>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D326" t="n">
+        <v>104</v>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>116</v>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>14:57:55</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
         <is>
           <t>16:56</t>
         </is>
       </c>
-      <c r="C319" t="inlineStr">
+      <c r="C328" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D319" t="n">
+      <c r="D328" t="n">
         <v>119</v>
       </c>
-      <c r="E319" t="inlineStr">
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D329" t="n">
+        <v>77</v>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D330" t="n">
+        <v>77</v>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>17:03</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D331" t="n">
+        <v>83</v>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>17:17</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>97</v>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
+        <v>104</v>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>114</v>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>115</v>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D336" t="n">
+        <v>116</v>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>118</v>
+      </c>
+      <c r="E337" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 84
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E337"/>
+  <dimension ref="A1:E347"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:40:34</t>
+          <t>Última actualización: 15:59:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 332</t>
+          <t>Total filas: 342</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -665,18 +665,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -686,11 +686,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -4036,7 +4036,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10:51:31</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4046,18 +4046,18 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>10:51:31</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4067,11 +4067,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E176" t="inlineStr"/>
     </row>
@@ -4225,7 +4225,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4235,11 +4235,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>108</v>
+        <v>20</v>
       </c>
       <c r="E184" t="inlineStr"/>
     </row>
@@ -4267,7 +4267,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4277,11 +4277,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="E186" t="inlineStr"/>
     </row>
@@ -4466,7 +4466,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D195" t="n">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -4901,7 +4901,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -4911,17 +4911,13 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>3</v>
-      </c>
-      <c r="E216" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -4936,7 +4932,7 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D217" t="n">
@@ -4947,7 +4943,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -4957,13 +4953,17 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>76</v>
-      </c>
-      <c r="E218" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -5161,7 +5161,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -5171,18 +5171,18 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="E228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -5192,11 +5192,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="E229" t="inlineStr"/>
     </row>
@@ -5626,7 +5626,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -5636,18 +5636,18 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="E249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -5657,11 +5657,11 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="E250" t="inlineStr"/>
     </row>
@@ -6681,7 +6681,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -6691,11 +6691,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -6706,7 +6706,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -6716,11 +6716,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7056,21 +7056,21 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -7081,21 +7081,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>16:03</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -7111,16 +7111,16 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:03</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -7131,21 +7131,21 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>16:16</t>
+          <t>16:04</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -7156,12 +7156,12 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -7170,7 +7170,7 @@
         </is>
       </c>
       <c r="D311" t="n">
-        <v>117</v>
+        <v>34</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -7181,21 +7181,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -7206,21 +7206,21 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>16:22</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -7231,21 +7231,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -7256,21 +7256,21 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>16:22</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -7281,21 +7281,21 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>16:25</t>
+          <t>16:24</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -7311,16 +7311,16 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>16:25</t>
+          <t>16:24</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -7331,12 +7331,12 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>16:26</t>
+          <t>16:25</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -7345,7 +7345,7 @@
         </is>
       </c>
       <c r="D318" t="n">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -7356,21 +7356,21 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>16:31</t>
+          <t>16:25</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>108</v>
+        <v>45</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -7386,16 +7386,16 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>16:32</t>
+          <t>16:26</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -7411,16 +7411,16 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:31</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -7431,21 +7431,21 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:32</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -7461,16 +7461,16 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -7481,21 +7481,21 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -7506,21 +7506,21 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>16:38</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -7531,12 +7531,12 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -7545,7 +7545,7 @@
         </is>
       </c>
       <c r="D326" t="n">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -7556,21 +7556,21 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:38</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -7586,16 +7586,16 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -7606,21 +7606,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:51</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -7631,21 +7631,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -7656,21 +7656,21 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -7686,16 +7686,16 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -7711,16 +7711,16 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -7736,16 +7736,16 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -7756,21 +7756,21 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -7781,21 +7781,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -7811,18 +7811,268 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
+          <t>17:17</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>97</v>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>104</v>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>17:27</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>88</v>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>114</v>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>115</v>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D342" t="n">
+        <v>116</v>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
           <t>17:38</t>
         </is>
       </c>
-      <c r="C337" t="inlineStr">
+      <c r="C343" t="inlineStr">
         <is>
           <t>17X38_ROMERO</t>
         </is>
       </c>
-      <c r="D337" t="n">
+      <c r="D343" t="n">
         <v>118</v>
       </c>
-      <c r="E337" t="inlineStr">
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D344" t="n">
+        <v>101</v>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>17:44</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>105</v>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>17:47</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D346" t="n">
+        <v>108</v>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>111</v>
+      </c>
+      <c r="E347" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7839,7 +8089,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7857,14 +8107,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:40:34</t>
+          <t>Última actualización: 15:59:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 87</t>
+          <t>Total filas: 90</t>
         </is>
       </c>
     </row>
@@ -8349,7 +8599,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -8370,7 +8620,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -8822,7 +9072,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -8832,18 +9082,18 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -8853,11 +9103,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E51" t="inlineStr"/>
     </row>
@@ -9809,6 +10059,81 @@
         <v>77</v>
       </c>
       <c r="E92" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>17:03</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>64</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>17:44</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>105</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>111</v>
+      </c>
+      <c r="E95" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9825,7 +10150,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E337"/>
+  <dimension ref="A1:E347"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9843,14 +10168,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:40:34</t>
+          <t>Última actualización: 15:59:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 332</t>
+          <t>Total filas: 342</t>
         </is>
       </c>
     </row>
@@ -10052,7 +10377,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -10062,18 +10387,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -10083,11 +10408,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -11175,7 +11500,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -11196,7 +11521,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -13433,7 +13758,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10:51:31</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -13443,18 +13768,18 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>10:51:31</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -13464,11 +13789,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E176" t="inlineStr"/>
     </row>
@@ -13622,7 +13947,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -13632,11 +13957,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>108</v>
+        <v>20</v>
       </c>
       <c r="E184" t="inlineStr"/>
     </row>
@@ -13664,7 +13989,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -13674,11 +13999,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="E186" t="inlineStr"/>
     </row>
@@ -13863,7 +14188,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D195" t="n">
@@ -13884,7 +14209,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -14298,7 +14623,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -14308,17 +14633,13 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>3</v>
-      </c>
-      <c r="E216" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -14333,7 +14654,7 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D217" t="n">
@@ -14344,7 +14665,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -14354,13 +14675,17 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>76</v>
-      </c>
-      <c r="E218" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -14558,7 +14883,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -14568,18 +14893,18 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="E228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -14589,11 +14914,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="E229" t="inlineStr"/>
     </row>
@@ -15023,7 +15348,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -15033,18 +15358,18 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="E249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -15054,11 +15379,11 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="E250" t="inlineStr"/>
     </row>
@@ -16078,7 +16403,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -16088,11 +16413,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -16103,7 +16428,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -16113,11 +16438,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -16453,21 +16778,21 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -16478,21 +16803,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>16:03</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -16508,16 +16833,16 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:03</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -16528,21 +16853,21 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>16:16</t>
+          <t>16:04</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -16553,12 +16878,12 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>14:23:38</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -16567,7 +16892,7 @@
         </is>
       </c>
       <c r="D311" t="n">
-        <v>117</v>
+        <v>34</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -16578,21 +16903,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -16603,21 +16928,21 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>14:23:38</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>16:22</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -16628,21 +16953,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -16653,21 +16978,21 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>16:22</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -16678,21 +17003,21 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>16:25</t>
+          <t>16:24</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -16708,16 +17033,16 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>16:25</t>
+          <t>16:24</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -16728,12 +17053,12 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>16:26</t>
+          <t>16:25</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -16742,7 +17067,7 @@
         </is>
       </c>
       <c r="D318" t="n">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -16753,21 +17078,21 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>16:31</t>
+          <t>16:25</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>108</v>
+        <v>45</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -16783,16 +17108,16 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>16:32</t>
+          <t>16:26</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -16808,16 +17133,16 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:31</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -16828,21 +17153,21 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:32</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -16858,16 +17183,16 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -16878,21 +17203,21 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -16903,21 +17228,21 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>16:38</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -16928,12 +17253,12 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -16942,7 +17267,7 @@
         </is>
       </c>
       <c r="D326" t="n">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -16953,21 +17278,21 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:38</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -16983,16 +17308,16 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -17003,21 +17328,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:51</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -17028,21 +17353,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -17053,21 +17378,21 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -17083,16 +17408,16 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -17108,16 +17433,16 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -17133,16 +17458,16 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -17153,21 +17478,21 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -17178,21 +17503,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -17208,18 +17533,268 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
+          <t>17:17</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>97</v>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>104</v>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>17:27</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>88</v>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>114</v>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>115</v>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D342" t="n">
+        <v>116</v>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
           <t>17:38</t>
         </is>
       </c>
-      <c r="C337" t="inlineStr">
+      <c r="C343" t="inlineStr">
         <is>
           <t>17X38_ROMERO</t>
         </is>
       </c>
-      <c r="D337" t="n">
+      <c r="D343" t="n">
         <v>118</v>
       </c>
-      <c r="E337" t="inlineStr">
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D344" t="n">
+        <v>101</v>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>17:44</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>105</v>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>17:47</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D346" t="n">
+        <v>108</v>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>111</v>
+      </c>
+      <c r="E347" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 85
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E347"/>
+  <dimension ref="A1:E356"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:59:48</t>
+          <t>Última actualización: 16:16:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 342</t>
+          <t>Total filas: 351</t>
         </is>
       </c>
     </row>
@@ -1852,7 +1852,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>06:58:06</t>
+          <t>07:31:04</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1862,18 +1862,18 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="E71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>07:31:04</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1883,11 +1883,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="E72" t="inlineStr"/>
     </row>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -2786,7 +2786,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -2944,7 +2944,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>07:51:22</t>
+          <t>08:22:12</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -2954,18 +2954,18 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="E123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>08:22:12</t>
+          <t>07:51:22</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -2975,11 +2975,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="E124" t="inlineStr"/>
     </row>
@@ -3175,7 +3175,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>08:57:53</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3185,18 +3185,18 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>08:57:53</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3206,11 +3206,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="E135" t="inlineStr"/>
     </row>
@@ -4372,7 +4372,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -4382,18 +4382,18 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="E191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -4403,11 +4403,11 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="E192" t="inlineStr"/>
     </row>
@@ -5287,7 +5287,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -5297,18 +5297,22 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>116</v>
-      </c>
-      <c r="E234" t="inlineStr"/>
+        <v>23</v>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -5318,17 +5322,13 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>23</v>
-      </c>
-      <c r="E235" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E235" t="inlineStr"/>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -5559,7 +5559,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>11:58:34</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -5569,18 +5569,22 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>113</v>
-      </c>
-      <c r="E246" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>11:58:34</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -5590,17 +5594,13 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>16</v>
-      </c>
-      <c r="E247" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="E247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -6081,7 +6081,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:46:01</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -6091,11 +6091,11 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -6106,7 +6106,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>12:46:01</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -6116,11 +6116,11 @@
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7456,7 +7456,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -7466,11 +7466,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -7481,7 +7481,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -7491,11 +7491,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -7606,21 +7606,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>16:51</t>
+          <t>16:44</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -7631,21 +7631,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:51</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>116</v>
+        <v>52</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -7661,16 +7661,16 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -7681,21 +7681,21 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:54</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -7706,21 +7706,21 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -7736,16 +7736,16 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -7756,21 +7756,21 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -7786,16 +7786,16 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -7811,16 +7811,16 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -7831,21 +7831,21 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>104</v>
+        <v>65</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -7856,12 +7856,12 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>17:27</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
@@ -7870,7 +7870,7 @@
         </is>
       </c>
       <c r="D339" t="n">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -7886,16 +7886,16 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -7911,16 +7911,16 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -7931,21 +7931,21 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:27</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -7956,21 +7956,21 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -7981,21 +7981,21 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D344" t="n">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8006,21 +8006,21 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8031,21 +8031,21 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -8056,23 +8056,248 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
+          <t>15:40:34</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>118</v>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
           <t>15:59:48</t>
         </is>
       </c>
-      <c r="B347" t="inlineStr">
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>101</v>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>17:44</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D349" t="n">
+        <v>105</v>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>17:46</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D350" t="n">
+        <v>90</v>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>17:47</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D351" t="n">
+        <v>108</v>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>17:48</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D352" t="n">
+        <v>92</v>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
         <is>
           <t>17:50</t>
         </is>
       </c>
-      <c r="C347" t="inlineStr">
+      <c r="C353" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D347" t="n">
+      <c r="D353" t="n">
         <v>111</v>
       </c>
-      <c r="E347" t="inlineStr">
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D354" t="n">
+        <v>95</v>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>18:03</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D355" t="n">
+        <v>107</v>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D356" t="n">
+        <v>108</v>
+      </c>
+      <c r="E356" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8089,7 +8314,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8107,14 +8332,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:59:48</t>
+          <t>Última actualización: 16:16:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 90</t>
+          <t>Total filas: 91</t>
         </is>
       </c>
     </row>
@@ -8599,7 +8824,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -8620,7 +8845,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -9072,7 +9297,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -9082,18 +9307,18 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -9103,11 +9328,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E51" t="inlineStr"/>
     </row>
@@ -10134,6 +10359,31 @@
         <v>111</v>
       </c>
       <c r="E95" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>95</v>
+      </c>
+      <c r="E96" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10150,7 +10400,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E347"/>
+  <dimension ref="A1:E349"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10168,14 +10418,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:59:48</t>
+          <t>Última actualización: 16:16:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 342</t>
+          <t>Total filas: 344</t>
         </is>
       </c>
     </row>
@@ -10377,7 +10627,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -10387,18 +10637,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -10408,11 +10658,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -11763,7 +12013,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>07:31:04</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -11773,18 +12023,18 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="E80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>07:31:04</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -11794,11 +12044,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="E81" t="inlineStr"/>
     </row>
@@ -12666,7 +12916,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>07:51:22</t>
+          <t>08:22:12</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -12676,18 +12926,18 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="E123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>08:22:12</t>
+          <t>07:51:22</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -12697,11 +12947,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="E124" t="inlineStr"/>
     </row>
@@ -12897,7 +13147,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>08:57:53</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -12907,18 +13157,18 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>08:57:53</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -12928,11 +13178,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="E135" t="inlineStr"/>
     </row>
@@ -15415,7 +15665,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -15425,22 +15675,18 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>26</v>
-      </c>
-      <c r="E252" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -15450,13 +15696,17 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>92</v>
-      </c>
-      <c r="E253" t="inlineStr"/>
+        <v>26</v>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -16203,7 +16453,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -16213,11 +16463,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -16228,7 +16478,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -16238,11 +16488,11 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -16453,7 +16703,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -16463,11 +16713,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -16503,7 +16753,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -16513,11 +16763,11 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -17013,7 +17263,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D316" t="n">
@@ -17038,7 +17288,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D317" t="n">
@@ -17128,46 +17378,46 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>16:31</t>
+          <t>16:26</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>108</v>
+        <v>10</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>16:32</t>
+          <t>16:31</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -17178,12 +17428,12 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:32</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -17192,7 +17442,7 @@
         </is>
       </c>
       <c r="D323" t="n">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -17203,7 +17453,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -17213,11 +17463,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -17228,12 +17478,12 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -17242,7 +17492,7 @@
         </is>
       </c>
       <c r="D325" t="n">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -17258,16 +17508,16 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -17278,21 +17528,21 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>16:38</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -17303,21 +17553,21 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:38</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -17328,21 +17578,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>16:51</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -17353,21 +17603,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:51</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>116</v>
+        <v>52</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -17383,16 +17633,16 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -17403,12 +17653,12 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -17417,7 +17667,7 @@
         </is>
       </c>
       <c r="D332" t="n">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -17438,7 +17688,7 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D333" t="n">
@@ -17458,16 +17708,16 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -17478,7 +17728,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
@@ -17488,11 +17738,11 @@
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -17508,16 +17758,16 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -17528,21 +17778,21 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -17553,46 +17803,46 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>17:27</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -17608,16 +17858,16 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -17628,21 +17878,21 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:27</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -17658,16 +17908,16 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -17683,16 +17933,16 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -17703,12 +17953,12 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
@@ -17717,7 +17967,7 @@
         </is>
       </c>
       <c r="D344" t="n">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -17728,21 +17978,21 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -17758,16 +18008,16 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -17783,18 +18033,68 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
+          <t>17:44</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>105</v>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>17:47</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>108</v>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
           <t>17:50</t>
         </is>
       </c>
-      <c r="C347" t="inlineStr">
+      <c r="C349" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D347" t="n">
+      <c r="D349" t="n">
         <v>111</v>
       </c>
-      <c r="E347" t="inlineStr">
+      <c r="E349" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 87
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E356"/>
+  <dimension ref="A1:E364"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:16:23</t>
+          <t>Última actualización: 16:22:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 351</t>
+          <t>Total filas: 359</t>
         </is>
       </c>
     </row>
@@ -1852,7 +1852,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>07:31:04</t>
+          <t>06:58:06</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1862,18 +1862,18 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="E71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>06:58:06</t>
+          <t>07:31:04</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1883,11 +1883,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="E72" t="inlineStr"/>
     </row>
@@ -2345,7 +2345,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D94" t="n">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D95" t="n">
@@ -3280,7 +3280,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>08:22:12</t>
+          <t>08:57:53</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -3290,18 +3290,18 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="E139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>08:57:53</t>
+          <t>08:22:12</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3311,11 +3311,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="E140" t="inlineStr"/>
     </row>
@@ -4183,7 +4183,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4193,18 +4193,18 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -4214,18 +4214,18 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>11:25:38</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4235,11 +4235,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="E184" t="inlineStr"/>
     </row>
@@ -4267,7 +4267,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>11:25:38</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4277,11 +4277,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>108</v>
+        <v>20</v>
       </c>
       <c r="E186" t="inlineStr"/>
     </row>
@@ -4466,7 +4466,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D195" t="n">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -4911,7 +4911,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -4922,7 +4922,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>11:45:06</t>
+          <t>12:58:39</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -4932,18 +4932,22 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>76</v>
-      </c>
-      <c r="E217" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>12:58:39</t>
+          <t>11:45:06</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -4953,17 +4957,13 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>3</v>
-      </c>
-      <c r="E218" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -5693,7 +5693,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>12:29:23</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -5703,22 +5703,18 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>26</v>
-      </c>
-      <c r="E252" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>12:29:23</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -5728,13 +5724,17 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>92</v>
-      </c>
-      <c r="E253" t="inlineStr"/>
+        <v>26</v>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -7281,12 +7281,12 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>16:22</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -7295,7 +7295,7 @@
         </is>
       </c>
       <c r="D316" t="n">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -7316,7 +7316,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D317" t="n">
@@ -7336,16 +7336,16 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>16:25</t>
+          <t>16:24</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D318" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -7356,7 +7356,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -7366,11 +7366,11 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -7386,16 +7386,16 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>16:26</t>
+          <t>16:25</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -7406,21 +7406,21 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>16:31</t>
+          <t>16:26</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -7431,21 +7431,21 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>16:32</t>
+          <t>16:31</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -7456,21 +7456,21 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:32</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -7481,7 +7481,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -7491,11 +7491,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -7511,16 +7511,16 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -7536,16 +7536,16 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -7556,21 +7556,21 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>16:38</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -7581,21 +7581,21 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:38</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -7606,21 +7606,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>16:44</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -7631,21 +7631,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>16:51</t>
+          <t>16:44</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -7656,21 +7656,21 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>116</v>
+        <v>28</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -7681,21 +7681,21 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>16:54</t>
+          <t>16:51</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -7711,16 +7711,16 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -7731,21 +7731,21 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:54</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -7756,12 +7756,12 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
@@ -7770,7 +7770,7 @@
         </is>
       </c>
       <c r="D335" t="n">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -7781,21 +7781,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -7811,16 +7811,16 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -7831,21 +7831,21 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:01</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -7856,21 +7856,21 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -7886,16 +7886,16 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -7906,21 +7906,21 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>104</v>
+        <v>65</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -7931,12 +7931,12 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>17:27</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
@@ -7945,7 +7945,7 @@
         </is>
       </c>
       <c r="D342" t="n">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -7956,21 +7956,21 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -7986,16 +7986,16 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D344" t="n">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8011,16 +8011,16 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8031,21 +8031,21 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:27</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -8056,21 +8056,21 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -8081,21 +8081,21 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -8106,21 +8106,21 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -8131,21 +8131,21 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -8156,21 +8156,21 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D351" t="n">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -8181,21 +8181,21 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D352" t="n">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -8211,16 +8211,16 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D353" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -8231,21 +8231,21 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -8256,21 +8256,21 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D355" t="n">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -8286,18 +8286,218 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
+          <t>17:46</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D356" t="n">
+        <v>90</v>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>16:22:52</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>17:46</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D357" t="n">
+        <v>84</v>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>17:47</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D358" t="n">
+        <v>108</v>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>17:48</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D359" t="n">
+        <v>92</v>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D360" t="n">
+        <v>111</v>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D361" t="n">
+        <v>95</v>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>16:22:52</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>18:02</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D362" t="n">
+        <v>100</v>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>18:03</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D363" t="n">
+        <v>107</v>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
           <t>18:04</t>
         </is>
       </c>
-      <c r="C356" t="inlineStr">
+      <c r="C364" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D356" t="n">
+      <c r="D364" t="n">
         <v>108</v>
       </c>
-      <c r="E356" t="inlineStr">
+      <c r="E364" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8332,7 +8532,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:16:23</t>
+          <t>Última actualización: 16:22:52</t>
         </is>
       </c>
     </row>
@@ -8824,7 +9024,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -8845,7 +9045,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -9297,7 +9497,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>10:35:49</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -9307,18 +9507,18 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>10:35:49</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -9328,11 +9528,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E51" t="inlineStr"/>
     </row>
@@ -10400,7 +10600,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E349"/>
+  <dimension ref="A1:E351"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10418,14 +10618,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:16:23</t>
+          <t>Última actualización: 16:22:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 344</t>
+          <t>Total filas: 346</t>
         </is>
       </c>
     </row>
@@ -10627,7 +10827,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:46:12</t>
+          <t>04:44:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -10637,18 +10837,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:44:55</t>
+          <t>03:46:12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -10658,11 +10858,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -12013,7 +12213,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>06:28:32</t>
+          <t>07:31:04</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -12023,18 +12223,18 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="E80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>07:31:04</t>
+          <t>06:28:32</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -12044,11 +12244,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="E81" t="inlineStr"/>
     </row>
@@ -12916,7 +13116,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>08:22:12</t>
+          <t>07:51:22</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -12926,18 +13126,18 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="E123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>07:51:22</t>
+          <t>08:22:12</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -12947,11 +13147,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="E124" t="inlineStr"/>
     </row>
@@ -13147,7 +13347,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>08:57:53</t>
+          <t>09:57:03</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -13157,18 +13357,18 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="E134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>09:57:03</t>
+          <t>08:57:53</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -13178,11 +13378,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E135" t="inlineStr"/>
     </row>
@@ -17263,7 +17463,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D316" t="n">
@@ -17278,7 +17478,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
@@ -17288,15 +17488,15 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>101</v>
+        <v>2</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -17308,16 +17508,16 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>16:25</t>
+          <t>16:24</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D318" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -17328,7 +17528,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -17338,11 +17538,11 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -17358,16 +17558,16 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>16:26</t>
+          <t>16:25</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -17378,7 +17578,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -17392,57 +17592,57 @@
         </is>
       </c>
       <c r="D321" t="n">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>16:31</t>
+          <t>16:26</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>108</v>
+        <v>10</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>16:32</t>
+          <t>16:31</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -17453,12 +17653,12 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:32</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -17467,7 +17667,7 @@
         </is>
       </c>
       <c r="D324" t="n">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -17478,7 +17678,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -17488,11 +17688,11 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -17503,12 +17703,12 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -17517,7 +17717,7 @@
         </is>
       </c>
       <c r="D326" t="n">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -17533,16 +17733,16 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -17553,21 +17753,21 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>16:38</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -17578,21 +17778,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:38</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -17603,21 +17803,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>16:51</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -17628,21 +17828,21 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:51</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>116</v>
+        <v>52</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -17658,16 +17858,16 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -17678,12 +17878,12 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
@@ -17692,7 +17892,7 @@
         </is>
       </c>
       <c r="D333" t="n">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -17713,7 +17913,7 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D334" t="n">
@@ -17733,16 +17933,16 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -17753,7 +17953,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
@@ -17763,11 +17963,11 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -17783,16 +17983,16 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -17803,50 +18003,50 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
@@ -17858,16 +18058,16 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -17878,21 +18078,21 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>17:27</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -17903,21 +18103,21 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:27</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -17933,16 +18133,16 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -17958,16 +18158,16 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D344" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -17983,16 +18183,16 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -18003,21 +18203,21 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -18033,16 +18233,16 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -18058,16 +18258,16 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -18083,20 +18283,70 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
+          <t>17:47</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D349" t="n">
+        <v>108</v>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
           <t>17:50</t>
         </is>
       </c>
-      <c r="C349" t="inlineStr">
+      <c r="C350" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D349" t="n">
+      <c r="D350" t="n">
         <v>111</v>
       </c>
-      <c r="E349" t="inlineStr">
-        <is>
-          <t>LP1912</t>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>16:22:52</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D351" t="n">
+        <v>119</v>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 89
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:28:40</t>
+          <t>Última actualización: 16:32:08</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 123</t>
+          <t>Total filas: 131</t>
         </is>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1322,7 +1322,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1712,7 +1712,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1722,11 +1722,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1762,7 +1762,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1772,11 +1772,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2462,7 +2462,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2472,11 +2472,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,12 +2512,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2526,7 +2526,7 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2542,16 +2542,16 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2562,21 +2562,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16:38</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,21 +2587,21 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:38</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2612,21 +2612,21 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16:44</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2637,12 +2637,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>16:44</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2662,21 +2662,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>16:51</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2687,21 +2687,21 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:51</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>116</v>
+        <v>52</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2712,12 +2712,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>16:54</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2726,7 +2726,7 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2737,21 +2737,21 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>16:28:39</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>16:55</t>
+          <t>16:54</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,21 +2762,21 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>16:28:39</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:55</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>119</v>
+        <v>27</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2787,21 +2787,21 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2822,7 +2822,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2837,21 +2837,21 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>17:01</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2862,21 +2862,21 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2887,21 +2887,21 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>17:01</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2917,16 +2917,16 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2937,21 +2937,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2962,21 +2962,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,21 +2987,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,21 +3012,21 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>104</v>
+        <v>51</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,21 +3037,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>17:27</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3062,21 +3062,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,21 +3087,21 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3112,21 +3112,21 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:25</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>114</v>
+        <v>53</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,21 +3137,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:27</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,21 +3162,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,21 +3187,21 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>118</v>
+        <v>71</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,21 +3212,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,21 +3237,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3262,21 +3262,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3287,21 +3287,21 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3312,21 +3312,21 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3342,16 +3342,16 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3362,21 +3362,21 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3387,21 +3387,21 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>16:28:39</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3412,21 +3412,21 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3442,16 +3442,16 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3467,16 +3467,16 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>18:02</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3487,21 +3487,21 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3517,16 +3517,16 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3542,18 +3542,218 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
+          <t>17:49</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>81</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>111</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>95</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>16:22:52</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>18:02</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>100</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>18:03</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>107</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>108</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>16:32:08</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>18:05</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>93</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>16:28:39</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
           <t>18:24</t>
         </is>
       </c>
-      <c r="C128" t="inlineStr">
+      <c r="C135" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D128" t="n">
+      <c r="D135" t="n">
         <v>116</v>
       </c>
-      <c r="E128" t="inlineStr">
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>16:32:08</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>113</v>
+      </c>
+      <c r="E136" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3570,7 +3770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3588,14 +3788,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:28:40</t>
+          <t>Última actualización: 16:32:08</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 27</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
     </row>
@@ -4254,21 +4454,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>111</v>
+        <v>73</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -4279,23 +4479,48 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>15:59:48</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>111</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>16:16:23</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B33" t="inlineStr">
         <is>
           <t>17:51</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D32" t="n">
+      <c r="D33" t="n">
         <v>95</v>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4312,7 +4537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4330,14 +4555,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:28:40</t>
+          <t>Última actualización: 16:32:08</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -4421,12 +4646,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:28:39</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -4435,7 +4660,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -4446,12 +4671,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:28:39</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -4460,7 +4685,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -4471,23 +4696,73 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>16:16:23</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>49</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>16:22:52</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>18:21</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
         <v>119</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>16:32:08</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>110</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 90
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E136"/>
+  <dimension ref="A1:E138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:32:08</t>
+          <t>Última actualización: 16:33:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 131</t>
+          <t>Total filas: 133</t>
         </is>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1322,7 +1322,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1712,7 +1712,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1722,11 +1722,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1737,7 +1737,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1747,11 +1747,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -3037,12 +3037,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:33:53</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:13</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3051,7 +3051,7 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3062,21 +3062,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3092,16 +3092,16 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3112,12 +3112,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>17:25</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3126,7 +3126,7 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,21 +3137,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>17:27</t>
+          <t>17:25</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,21 +3162,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:27</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,12 +3187,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3201,7 +3201,7 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,21 +3212,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,21 +3237,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3262,7 +3262,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -3272,11 +3272,11 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3292,16 +3292,16 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3317,16 +3317,16 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3337,21 +3337,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3367,16 +3367,16 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3387,12 +3387,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -3401,7 +3401,7 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3412,7 +3412,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3422,11 +3422,11 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3437,12 +3437,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -3451,7 +3451,7 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3462,7 +3462,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3472,11 +3472,11 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3487,21 +3487,21 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3512,21 +3512,21 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3537,12 +3537,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>16:28:39</t>
+          <t>16:33:53</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3551,7 +3551,7 @@
         </is>
       </c>
       <c r="D128" t="n">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,21 +3562,21 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3587,21 +3587,21 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:28:39</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,21 +3612,21 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>18:02</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3642,16 +3642,16 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3662,21 +3662,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:02</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3687,21 +3687,21 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3712,21 +3712,21 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>16:28:39</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3742,18 +3742,68 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
+          <t>18:05</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>93</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>16:28:39</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>116</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>16:32:08</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
           <t>18:25</t>
         </is>
       </c>
-      <c r="C136" t="inlineStr">
+      <c r="C138" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D136" t="n">
+      <c r="D138" t="n">
         <v>113</v>
       </c>
-      <c r="E136" t="inlineStr">
+      <c r="E138" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3788,7 +3838,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:32:08</t>
+          <t>Última actualización: 16:33:54</t>
         </is>
       </c>
     </row>
@@ -4537,7 +4587,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4555,14 +4605,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:32:08</t>
+          <t>Última actualización: 16:33:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -4646,12 +4696,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>16:33:53</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>17:02</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -4660,7 +4710,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -4671,12 +4721,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>16:28:39</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -4685,7 +4735,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -4696,12 +4746,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:28:39</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -4710,7 +4760,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -4721,12 +4771,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -4735,7 +4785,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -4746,23 +4796,48 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>16:22:52</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>119</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>16:32:08</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>18:22</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D13" t="n">
         <v>110</v>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 91
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E138"/>
+  <dimension ref="A1:E139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:33:54</t>
+          <t>Última actualización: 16:34:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 133</t>
+          <t>Total filas: 134</t>
         </is>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1322,7 +1322,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1737,7 +1737,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1747,11 +1747,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,7 +1762,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1772,11 +1772,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2462,7 +2462,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>14:43:48</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2472,11 +2472,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>14:57:55</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>14:57:55</t>
+          <t>14:43:48</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2522,11 +2522,11 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2912,21 +2912,21 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:34:35</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>17:02</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2967,16 +2967,16 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,12 +2987,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,21 +3012,21 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,21 +3037,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>16:33:53</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>17:13</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3062,12 +3062,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:33:53</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:13</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3076,7 +3076,7 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,21 +3087,21 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3117,16 +3117,16 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,12 +3137,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>17:25</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3151,7 +3151,7 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,21 +3162,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>17:27</t>
+          <t>17:25</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,21 +3187,21 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:27</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,12 +3212,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3226,7 +3226,7 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,21 +3237,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3262,21 +3262,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3287,7 +3287,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3297,11 +3297,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3317,16 +3317,16 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3342,16 +3342,16 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3362,21 +3362,21 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3392,16 +3392,16 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3412,12 +3412,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3426,7 +3426,7 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3437,7 +3437,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3447,11 +3447,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3462,12 +3462,12 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -3476,7 +3476,7 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3487,7 +3487,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3497,11 +3497,11 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3512,21 +3512,21 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>16:33:53</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,12 +3562,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:33:53</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -3576,7 +3576,7 @@
         </is>
       </c>
       <c r="D129" t="n">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3587,12 +3587,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>16:28:39</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3601,7 +3601,7 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,21 +3612,21 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:28:39</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3637,12 +3637,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3651,7 +3651,7 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3662,21 +3662,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>18:02</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3687,12 +3687,12 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:02</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -3701,7 +3701,7 @@
         </is>
       </c>
       <c r="D134" t="n">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3717,16 +3717,16 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,12 +3737,12 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -3751,7 +3751,7 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3762,21 +3762,21 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>16:28:39</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,23 +3787,48 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
+          <t>16:28:39</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>116</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
           <t>16:32:08</t>
         </is>
       </c>
-      <c r="B138" t="inlineStr">
+      <c r="B139" t="inlineStr">
         <is>
           <t>18:25</t>
         </is>
       </c>
-      <c r="C138" t="inlineStr">
+      <c r="C139" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D138" t="n">
+      <c r="D139" t="n">
         <v>113</v>
       </c>
-      <c r="E138" t="inlineStr">
+      <c r="E139" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3838,7 +3863,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:33:54</t>
+          <t>Última actualización: 16:34:35</t>
         </is>
       </c>
     </row>
@@ -4605,7 +4630,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:33:54</t>
+          <t>Última actualización: 16:34:35</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 92
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:34:35</t>
+          <t>Última actualización: 16:41:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 134</t>
+          <t>Total filas: 137</t>
         </is>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1322,7 +1322,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1712,7 +1712,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>13:54:15</t>
+          <t>13:35:25</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1722,11 +1722,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1762,7 +1762,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>13:35:25</t>
+          <t>13:54:15</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1772,11 +1772,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3062,21 +3062,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>16:33:53</t>
+          <t>16:41:15</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>17:13</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,12 +3087,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:33:53</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:13</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3101,7 +3101,7 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3112,21 +3112,21 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3142,16 +3142,16 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,12 +3162,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>17:25</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3176,7 +3176,7 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,21 +3187,21 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>17:27</t>
+          <t>17:25</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,21 +3212,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:27</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,12 +3237,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3251,7 +3251,7 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3262,21 +3262,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3287,21 +3287,21 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3312,7 +3312,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>15:40:34</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3322,11 +3322,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3342,16 +3342,16 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3367,16 +3367,16 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3387,21 +3387,21 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>15:40:34</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3417,16 +3417,16 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3437,12 +3437,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -3451,7 +3451,7 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3487,21 +3487,21 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3512,7 +3512,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3522,11 +3522,11 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3537,21 +3537,21 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>16:33:53</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3587,12 +3587,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:33:53</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3601,7 +3601,7 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,12 +3612,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>16:28:39</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3626,7 +3626,7 @@
         </is>
       </c>
       <c r="D131" t="n">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3637,21 +3637,21 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>15:59:48</t>
+          <t>16:28:39</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3662,12 +3662,12 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>15:59:48</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -3676,7 +3676,7 @@
         </is>
       </c>
       <c r="D133" t="n">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3687,21 +3687,21 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>18:02</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3712,12 +3712,12 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:22:52</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:02</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -3726,7 +3726,7 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3742,16 +3742,16 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3762,12 +3762,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -3776,7 +3776,7 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,21 +3787,21 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>16:28:39</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3812,23 +3812,98 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
+          <t>16:28:39</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>116</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
           <t>16:32:08</t>
         </is>
       </c>
-      <c r="B139" t="inlineStr">
+      <c r="B140" t="inlineStr">
         <is>
           <t>18:25</t>
         </is>
       </c>
-      <c r="C139" t="inlineStr">
+      <c r="C140" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D139" t="n">
+      <c r="D140" t="n">
         <v>113</v>
       </c>
-      <c r="E139" t="inlineStr">
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>16:41:15</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>18:34</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>113</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>16:41:15</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>18:38</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>117</v>
+      </c>
+      <c r="E142" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3863,7 +3938,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:34:35</t>
+          <t>Última actualización: 16:41:15</t>
         </is>
       </c>
     </row>
@@ -4612,7 +4687,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4630,14 +4705,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:34:35</t>
+          <t>Última actualización: 16:41:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 9</t>
         </is>
       </c>
     </row>
@@ -4721,12 +4796,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:33:53</t>
+          <t>16:41:15</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17:02</t>
+          <t>17:01</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -4735,7 +4810,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -4746,12 +4821,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>16:32:08</t>
+          <t>16:33:53</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>17:02</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -4760,7 +4835,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -4771,12 +4846,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>16:28:39</t>
+          <t>16:32:08</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -4785,7 +4860,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -4796,12 +4871,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>16:16:23</t>
+          <t>16:28:39</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -4810,7 +4885,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -4821,12 +4896,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>16:22:52</t>
+          <t>16:16:23</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -4835,7 +4910,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -4846,23 +4921,48 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>16:22:52</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>119</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>16:32:08</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>18:22</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D14" t="n">
         <v>110</v>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 95
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -439,14 +439,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912 - 10/01/2026</t>
+          <t>LÍNEA 141 - LP1912</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Actualización: 16:43:55</t>
+          <t>10/01 16:46:42</t>
         </is>
       </c>
     </row>
@@ -487,21 +487,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16:51</t>
+          <t>16:47</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -512,7 +512,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -537,7 +537,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -576,7 +576,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -587,7 +587,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -601,7 +601,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -612,7 +612,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -637,7 +637,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -651,7 +651,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -662,12 +662,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>17:11</t>
+          <t>17:13</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -687,12 +687,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>17:13</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -701,7 +701,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -712,7 +712,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -737,21 +737,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:23</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -762,21 +762,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>17:27</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -801,7 +801,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -812,7 +812,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -837,7 +837,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -851,7 +851,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -862,12 +862,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -887,7 +887,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -912,7 +912,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -926,7 +926,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -951,7 +951,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,7 +962,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -976,7 +976,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -987,12 +987,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>18:33</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1012,7 +1012,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1037,7 +1037,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1051,7 +1051,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1081,14 +1081,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912-215 - 10/01/2026</t>
+          <t>LÍNEA 141 - LP1912-215</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Actualización: 16:43:55</t>
+          <t>10/01 16:46:42</t>
         </is>
       </c>
     </row>
@@ -1129,7 +1129,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1143,7 +1143,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1154,7 +1154,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1168,7 +1168,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1179,7 +1179,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1193,7 +1193,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1223,14 +1223,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - 6203-6173 - 10/01/2026</t>
+          <t>LÍNEA 141 - 6203-6173</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Actualización: 16:43:55</t>
+          <t>10/01 16:46:42</t>
         </is>
       </c>
     </row>
@@ -1271,12 +1271,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16:58</t>
+          <t>16:59</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1285,7 +1285,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1296,7 +1296,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:43:55</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 96
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,21 +439,21 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912</t>
+          <t>LÍNEA 141 - LP1912 - 10/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>10/01 16:46:42</t>
+          <t>Última actualización: 16:50:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Filas: 23</t>
+          <t>Total filas: 29</t>
         </is>
       </c>
     </row>
@@ -512,12 +512,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -537,21 +537,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:51</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -567,16 +567,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>17:01</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -592,16 +592,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -617,16 +617,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:01</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -642,16 +642,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -667,16 +667,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>17:13</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -692,16 +692,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -717,16 +717,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:13</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -742,16 +742,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>17:23</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -767,16 +767,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -787,21 +787,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -817,16 +817,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:23</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -842,16 +842,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -862,21 +862,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -892,16 +892,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -917,16 +917,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>18:02</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -942,16 +942,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,21 +962,21 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -992,16 +992,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>18:34</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1012,21 +1012,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>18:38</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1042,18 +1042,168 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>64</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>18:02</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>76</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>78</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>98</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>18:34</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>108</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>18:38</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>112</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>18:41</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="D34" t="n">
         <v>115</v>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1081,21 +1231,21 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912-215</t>
+          <t>LÍNEA 141 - LP1912-215 - 10/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>10/01 16:46:42</t>
+          <t>Última actualización: 16:50:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Filas: 3</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -1212,7 +1362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1223,21 +1373,21 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - 6203-6173</t>
+          <t>LÍNEA 141 - 6203-6173 - 10/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>10/01 16:46:42</t>
+          <t>Última actualización: 16:50:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Filas: 2</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -1271,12 +1421,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16:59</t>
+          <t>16:58</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1285,7 +1435,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1301,18 +1451,43 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>16:59</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>13</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>18:21</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D8" t="n">
         <v>95</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 97
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:50:41</t>
+          <t>Última actualización: 16:52:37</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 29</t>
+          <t>Total filas: 35</t>
         </is>
       </c>
     </row>
@@ -562,7 +562,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -572,11 +572,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -592,16 +592,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -617,16 +617,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>17:01</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -642,16 +642,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>17:01</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -667,16 +667,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -692,16 +692,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -717,16 +717,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>17:13</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -742,16 +742,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:13</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -767,16 +767,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>16:50:41</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -797,11 +797,11 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -812,21 +812,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>17:23</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -837,21 +837,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -862,21 +862,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>16:50:41</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:23</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -892,16 +892,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -912,21 +912,21 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -942,16 +942,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,21 +962,21 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>16:50:41</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -992,16 +992,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1012,21 +1012,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>16:50:41</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1037,21 +1037,21 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1067,16 +1067,16 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>18:02</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1087,21 +1087,21 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1117,16 +1117,16 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1137,21 +1137,21 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>18:34</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1167,16 +1167,16 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>18:38</t>
+          <t>18:02</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,23 +1187,173 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>18:03</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>71</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>78</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>16:52:37</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>18:14</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>82</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>98</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>18:34</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>108</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>18:38</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>112</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>18:41</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="D40" t="n">
         <v>115</v>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1220,7 +1370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1238,14 +1388,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:50:41</t>
+          <t>Última actualización: 16:52:37</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -1346,6 +1496,31 @@
         <v>64</v>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>16:52:37</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>59</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1362,7 +1537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1380,14 +1555,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:50:41</t>
+          <t>Última actualización: 16:52:37</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -1421,12 +1596,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:50:41</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16:58</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1435,7 +1610,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1446,12 +1621,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16:59</t>
+          <t>16:58</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1460,7 +1635,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1476,18 +1651,43 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>16:59</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>13</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>18:21</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D9" t="n">
         <v>95</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 98
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:52:37</t>
+          <t>Última actualización: 17:13:30</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 35</t>
+          <t>Total filas: 44</t>
         </is>
       </c>
     </row>
@@ -787,21 +787,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -837,21 +837,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -862,21 +862,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>17:23</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -892,16 +892,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:23</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -912,21 +912,21 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>16:50:41</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,21 +937,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:27</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,21 +962,21 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -987,21 +987,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1017,16 +1017,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1037,21 +1037,21 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>16:50:41</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1062,12 +1062,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1076,7 +1076,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1087,21 +1087,21 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>16:50:41</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1112,21 +1112,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:41</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1137,21 +1137,21 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1162,21 +1162,21 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>18:02</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,21 +1187,21 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1212,21 +1212,21 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1237,21 +1237,21 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>18:14</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1262,21 +1262,21 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1292,16 +1292,16 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>18:34</t>
+          <t>18:02</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1312,21 +1312,21 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>18:38</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1342,18 +1342,243 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>78</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>16:52:37</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>18:14</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>82</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>98</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>17:13:30</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>74</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>18:34</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>108</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>18:38</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>112</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
           <t>18:41</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D40" t="n">
+      <c r="D46" t="n">
         <v>115</v>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>17:13:30</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>18:41</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>88</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>17:13:30</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>19:01</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>108</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>17:13:30</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>118</v>
+      </c>
+      <c r="E49" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1388,7 +1613,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:52:37</t>
+          <t>Última actualización: 17:13:30</t>
         </is>
       </c>
     </row>
@@ -1537,7 +1762,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1555,14 +1780,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:52:37</t>
+          <t>Última actualización: 17:13:30</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -1690,6 +1915,56 @@
       <c r="E9" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>17:13:30</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>69</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>17:13:30</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>118</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 99
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:13:30</t>
+          <t>Última actualización: 17:35:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 44</t>
+          <t>Total filas: 58</t>
         </is>
       </c>
     </row>
@@ -812,7 +812,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>16:50:41</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -822,11 +822,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -837,7 +837,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -847,11 +847,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1112,21 +1112,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>17:41</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1137,21 +1137,21 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:41</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1162,21 +1162,21 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>16:50:41</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,21 +1187,21 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1217,16 +1217,16 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1242,16 +1242,16 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1262,17 +1262,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1292,16 +1292,16 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>18:02</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1317,16 +1317,16 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1337,21 +1337,21 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1362,21 +1362,21 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>18:14</t>
+          <t>18:02</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1387,21 +1387,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1412,21 +1412,21 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1442,16 +1442,16 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>18:34</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1462,21 +1462,21 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>18:38</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>112</v>
+        <v>30</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1487,21 +1487,21 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:14</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1512,21 +1512,21 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:24</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1537,21 +1537,21 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1567,18 +1567,368 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>74</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>18:31</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>56</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>18:34</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>108</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>18:38</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>112</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>17:13:30</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>18:41</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>88</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>18:41</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>115</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>18:45</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>70</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>18:51</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>76</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>84</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>17:13:30</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>19:01</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>108</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>17:13:30</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
           <t>19:11</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C59" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D49" t="n">
+      <c r="D59" t="n">
         <v>118</v>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>19:19</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>104</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>106</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>19:29</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>114</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>116</v>
+      </c>
+      <c r="E63" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1595,7 +1945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1613,14 +1963,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:13:30</t>
+          <t>Última actualización: 17:35:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -1704,21 +2054,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1729,23 +2079,98 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>64</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>16:52:37</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>17:51</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>59</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>106</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>116</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1780,7 +2205,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:13:30</t>
+          <t>Última actualización: 17:35:09</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 100
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:35:09</t>
+          <t>Última actualización: 17:47:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 58</t>
+          <t>Total filas: 66</t>
         </is>
       </c>
     </row>
@@ -1337,21 +1337,21 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1362,21 +1362,21 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>18:02</t>
+          <t>17:54</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1392,16 +1392,16 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1412,12 +1412,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:02</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1426,7 +1426,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1437,21 +1437,21 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1462,21 +1462,21 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1487,21 +1487,21 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>18:14</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1512,21 +1512,21 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1537,21 +1537,21 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:14</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1562,21 +1562,21 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1587,21 +1587,21 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>18:24</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1612,21 +1612,21 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>18:34</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1637,21 +1637,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>18:38</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1662,21 +1662,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1687,21 +1687,21 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>115</v>
+        <v>56</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1712,21 +1712,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1737,21 +1737,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>18:38</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,21 +1762,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1787,21 +1787,21 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,21 +1812,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>18:44</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>118</v>
+        <v>57</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1842,16 +1842,16 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>19:19</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1867,16 +1867,16 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1892,16 +1892,16 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,23 +1912,223 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
+          <t>17:13:30</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>19:01</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>108</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>17:13:30</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>118</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>17:47:22</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>90</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
           <t>17:35:09</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>19:19</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>104</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>106</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>19:29</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>114</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
         <is>
           <t>19:31</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D63" t="n">
+      <c r="D69" t="n">
         <v>116</v>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>17:47:22</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>113</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>17:47:22</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>19:44</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>117</v>
+      </c>
+      <c r="E71" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1940,6 +2140,273 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - LP1912-215 - 10/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 17:47:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>17:44</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>58</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>64</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>16:52:37</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>59</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>17:47:22</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>106</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>116</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1956,14 +2423,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912-215 - 10/01/2026</t>
+          <t>LÍNEA 141 - 6203-6173 - 10/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:35:09</t>
+          <t>Última actualización: 17:47:22</t>
         </is>
       </c>
     </row>
@@ -2004,75 +2471,75 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>16:58</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>16:59</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
@@ -2084,310 +2551,93 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>18:22</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="E12" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - 6203-6173 - 10/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 17:35:09</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>16:52:37</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>16:57</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>5</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>16:50:41</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>16:58</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>8</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>16:46:42</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>16:59</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>13</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>16:46:42</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>18:21</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>95</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>17:13:30</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>18:22</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>69</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>17:13:30</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>19:11</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>118</v>
-      </c>
-      <c r="E11" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 101
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:47:22</t>
+          <t>Última actualización: 17:54:43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 66</t>
+          <t>Total filas: 72</t>
         </is>
       </c>
     </row>
@@ -1712,21 +1712,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>18:34</t>
+          <t>18:33</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>108</v>
+        <v>39</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1742,16 +1742,16 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>18:38</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,21 +1762,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:38</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1787,7 +1787,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1797,11 +1797,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,21 +1812,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>18:44</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1837,12 +1837,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>18:44</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1851,7 +1851,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1867,16 +1867,16 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1892,16 +1892,16 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,21 +1912,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>18:53</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1937,21 +1937,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,21 +1962,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1987,21 +1987,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>19:19</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2012,21 +2012,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2042,16 +2042,16 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:19</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2062,21 +2062,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2087,21 +2087,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2112,23 +2112,173 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>19:29</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>114</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>17:54:43</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>96</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>17:54:43</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>96</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>116</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
           <t>17:47:22</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>113</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>17:47:22</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
         <is>
           <t>19:44</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="C76" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D71" t="n">
+      <c r="D76" t="n">
         <v>117</v>
       </c>
-      <c r="E71" t="inlineStr">
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>17:54:43</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>117</v>
+      </c>
+      <c r="E77" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2145,7 +2295,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2163,14 +2313,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:47:22</t>
+          <t>Última actualización: 17:54:43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 10</t>
         </is>
       </c>
     </row>
@@ -2354,12 +2504,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2368,7 +2518,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2384,18 +2534,68 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>106</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>17:54:43</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>96</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>19:31</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D15" t="n">
         <v>116</v>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2430,7 +2630,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:47:22</t>
+          <t>Última actualización: 17:54:43</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 102
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:54:43</t>
+          <t>Última actualización: 18:10:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 72</t>
+          <t>Total filas: 79</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1447,11 +1447,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1462,7 +1462,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1472,11 +1472,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1537,12 +1537,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>18:14</t>
+          <t>18:11</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1551,7 +1551,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1562,12 +1562,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:11</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1576,7 +1576,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1587,21 +1587,21 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>18:14</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1612,21 +1612,21 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1637,21 +1637,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:24</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1662,21 +1662,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1687,21 +1687,21 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1712,21 +1712,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>18:33</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1737,21 +1737,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>18:34</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,21 +1762,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>18:38</t>
+          <t>18:33</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>112</v>
+        <v>39</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1787,21 +1787,21 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1817,16 +1817,16 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:38</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1837,12 +1837,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>18:44</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1851,7 +1851,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1862,21 +1862,21 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1887,21 +1887,21 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>18:44</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,21 +1912,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>18:53</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1942,16 +1942,16 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,21 +1962,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>18:53</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1987,21 +1987,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2012,21 +2012,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2037,21 +2037,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>19:19</t>
+          <t>19:03</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2062,21 +2062,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2087,21 +2087,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:14</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2112,21 +2112,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2137,21 +2137,21 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:19</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2167,16 +2167,16 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2192,16 +2192,16 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2212,21 +2212,21 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2237,21 +2237,21 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>19:44</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2267,18 +2267,193 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>96</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>116</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>18:10:41</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>81</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>17:47:22</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>113</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>17:47:22</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>19:44</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>117</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>17:54:43</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
           <t>19:51</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
+      <c r="C82" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D77" t="n">
+      <c r="D82" t="n">
         <v>117</v>
       </c>
-      <c r="E77" t="inlineStr">
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>18:10:41</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>19:58</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>108</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>18:10:41</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>110</v>
+      </c>
+      <c r="E84" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2295,7 +2470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2313,14 +2488,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:54:43</t>
+          <t>Última actualización: 18:10:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 10</t>
+          <t>Total filas: 11</t>
         </is>
       </c>
     </row>
@@ -2596,6 +2771,31 @@
         <v>116</v>
       </c>
       <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>18:10:41</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>110</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2612,7 +2812,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2630,14 +2830,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:54:43</t>
+          <t>Última actualización: 18:10:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -2838,6 +3038,31 @@
         <v>85</v>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>18:10:41</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>19:15</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>65</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 103
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:10:41</t>
+          <t>Última actualización: 18:31:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 79</t>
+          <t>Total filas: 87</t>
         </is>
       </c>
     </row>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2062,21 +2062,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>118</v>
+        <v>34</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2087,21 +2087,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>19:14</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2112,21 +2112,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:14</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2137,12 +2137,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>19:19</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2151,7 +2151,7 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2162,21 +2162,21 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:19</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2187,12 +2187,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2201,7 +2201,7 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2217,16 +2217,16 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2237,21 +2237,21 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2272,7 +2272,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D77" t="n">
@@ -2287,21 +2287,21 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2312,7 +2312,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2322,11 +2322,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2337,21 +2337,21 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:31</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2362,21 +2362,21 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>19:44</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>117</v>
+        <v>63</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2387,21 +2387,21 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2412,21 +2412,21 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>19:58</t>
+          <t>19:44</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2437,23 +2437,223 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>19:46</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>75</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>17:54:43</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>117</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
           <t>18:10:41</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>19:58</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>108</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>88</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>18:10:41</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
         <is>
           <t>20:00</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
+      <c r="C88" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D84" t="n">
+      <c r="D88" t="n">
         <v>110</v>
       </c>
-      <c r="E84" t="inlineStr">
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>90</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>20:14</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>103</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>20:26</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>115</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>20:29</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>118</v>
+      </c>
+      <c r="E92" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2470,7 +2670,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2488,14 +2688,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:10:41</t>
+          <t>Última actualización: 18:31:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 11</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -2796,6 +2996,31 @@
         <v>110</v>
       </c>
       <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>90</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2812,7 +3037,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2830,14 +3055,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:10:41</t>
+          <t>Última actualización: 18:31:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 9</t>
         </is>
       </c>
     </row>
@@ -3046,23 +3271,48 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>19:13</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>42</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>18:10:41</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>19:15</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D14" t="n">
         <v>65</v>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 104
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:31:18</t>
+          <t>Última actualización: 18:44:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 87</t>
+          <t>Total filas: 92</t>
         </is>
       </c>
     </row>
@@ -1312,7 +1312,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1322,11 +1322,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1347,11 +1347,11 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1937,21 +1937,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,21 +1962,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>18:53</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1987,21 +1987,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:53</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2012,21 +2012,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2037,21 +2037,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>19:03</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2062,21 +2062,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:03</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2087,21 +2087,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>118</v>
+        <v>34</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2112,21 +2112,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>19:14</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2137,21 +2137,21 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:14</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2162,12 +2162,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>19:19</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2176,7 +2176,7 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2187,21 +2187,21 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2217,16 +2217,16 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:19</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2237,21 +2237,21 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2262,21 +2262,21 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2287,12 +2287,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:26</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2301,7 +2301,7 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2317,16 +2317,16 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2337,21 +2337,21 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2362,21 +2362,21 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2387,21 +2387,21 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:31</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2412,21 +2412,21 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>19:44</t>
+          <t>19:31</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2437,21 +2437,21 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>19:46</t>
+          <t>19:33</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2462,21 +2462,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>117</v>
+        <v>63</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2487,21 +2487,21 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>19:58</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,21 +2512,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:44</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2537,21 +2537,21 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:46</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2562,21 +2562,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,21 +2587,21 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>20:14</t>
+          <t>19:58</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2617,16 +2617,16 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>20:26</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2637,23 +2637,148 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
+          <t>18:10:41</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>110</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
           <t>18:31:18</t>
         </is>
       </c>
-      <c r="B92" t="inlineStr">
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>90</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>20:14</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>103</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>20:26</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>115</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>18:44:34</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>20:28</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>104</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
         <is>
           <t>20:29</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr">
+      <c r="C97" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D92" t="n">
+      <c r="D97" t="n">
         <v>118</v>
       </c>
-      <c r="E92" t="inlineStr">
+      <c r="E97" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2688,7 +2813,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:31:18</t>
+          <t>Última actualización: 18:44:34</t>
         </is>
       </c>
     </row>
@@ -3037,7 +3162,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3055,14 +3180,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:31:18</t>
+          <t>Última actualización: 18:44:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 9</t>
+          <t>Total filas: 10</t>
         </is>
       </c>
     </row>
@@ -3315,6 +3440,31 @@
       <c r="E14" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>18:44:34</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>20:41</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>117</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 105
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:44:34</t>
+          <t>Última actualización: 18:52:04</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 92</t>
+          <t>Total filas: 97</t>
         </is>
       </c>
     </row>
@@ -1987,21 +1987,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>18:53</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2012,21 +2012,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:53</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2037,21 +2037,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2062,21 +2062,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>19:03</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2087,21 +2087,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:03</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2112,21 +2112,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>118</v>
+        <v>12</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2137,21 +2137,21 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>19:14</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2162,21 +2162,21 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2187,21 +2187,21 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>18:44:34</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:14</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2212,21 +2212,21 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>19:19</t>
+          <t>19:15</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>104</v>
+        <v>23</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2237,21 +2237,21 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2262,21 +2262,21 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2287,12 +2287,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>18:44:34</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>19:26</t>
+          <t>19:19</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2301,7 +2301,7 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>42</v>
+        <v>104</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2312,21 +2312,21 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2337,21 +2337,21 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2362,12 +2362,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:26</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2376,7 +2376,7 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2392,16 +2392,16 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2412,12 +2412,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2426,7 +2426,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2437,21 +2437,21 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>18:44:34</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>19:33</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2462,21 +2462,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:31</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2487,21 +2487,21 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:31</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,21 +2512,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>19:44</t>
+          <t>19:33</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>117</v>
+        <v>49</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2542,16 +2542,16 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>19:46</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2562,21 +2562,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,21 +2587,21 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>19:58</t>
+          <t>19:44</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2617,16 +2617,16 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:46</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2637,21 +2637,21 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2662,21 +2662,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>19:58</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2692,16 +2692,16 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>20:14</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2712,21 +2712,21 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>20:26</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2737,21 +2737,21 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>18:44:34</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>20:28</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2767,18 +2767,143 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
+          <t>20:14</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>103</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>20:26</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>115</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>18:44:34</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>20:28</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>104</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
           <t>20:29</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
+      <c r="C100" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D97" t="n">
+      <c r="D100" t="n">
         <v>118</v>
       </c>
-      <c r="E97" t="inlineStr">
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>18:52:04</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>20:44</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>112</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>18:52:04</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>113</v>
+      </c>
+      <c r="E102" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2790,6 +2915,398 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - LP1912-215 - 10/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 18:52:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 13</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>17:44</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>58</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>16:46:42</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>64</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>16:52:37</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>59</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>17:47:22</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>17:54:43</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>19:20</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>86</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>106</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>17:54:43</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>96</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>17:35:09</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>116</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>18:10:41</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>110</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>90</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>18:52:04</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>20:44</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>112</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2806,14 +3323,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912-215 - 10/01/2026</t>
+          <t>LÍNEA 141 - 6203-6173 - 10/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:44:34</t>
+          <t>Última actualización: 18:52:04</t>
         </is>
       </c>
     </row>
@@ -2854,75 +3371,75 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>16:58</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>16:59</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
@@ -2934,535 +3451,218 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>18:22</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>118</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:13</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:14</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:15</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>20:41</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>20:42</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="E17" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - 6203-6173 - 10/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 18:44:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 10</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>16:52:37</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>16:57</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>5</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>16:50:41</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>16:58</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>8</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>16:46:42</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>16:59</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>13</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>16:46:42</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>18:21</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>95</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>17:13:30</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>18:22</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>69</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>17:13:30</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>19:11</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>118</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>17:47:22</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>19:12</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>85</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>18:31:18</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>19:13</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>42</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>18:10:41</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>19:15</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>65</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>18:44:34</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>20:41</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>117</v>
-      </c>
-      <c r="E15" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 106
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:52:04</t>
+          <t>Última actualización: 19:11:59</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 97</t>
+          <t>Total filas: 111</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>17:13:30</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1847,11 +1847,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1862,7 +1862,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>17:13:30</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1872,11 +1872,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2362,12 +2362,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>18:44:34</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>19:26</t>
+          <t>19:22</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2376,7 +2376,7 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2387,21 +2387,21 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:26</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>114</v>
+        <v>42</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2412,21 +2412,21 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2437,21 +2437,21 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2462,21 +2462,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2487,21 +2487,21 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,21 +2512,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>18:44:34</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>19:33</t>
+          <t>19:31</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2537,21 +2537,21 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:31</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2562,21 +2562,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:33</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>113</v>
+        <v>49</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,21 +2587,21 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>19:44</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>117</v>
+        <v>63</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2612,21 +2612,21 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>19:46</t>
+          <t>19:38</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2637,21 +2637,21 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>117</v>
+        <v>28</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2662,21 +2662,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>19:58</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2687,21 +2687,21 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2712,21 +2712,21 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:43</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2737,21 +2737,21 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>19:44</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2767,7 +2767,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>20:14</t>
+          <t>19:46</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2776,7 +2776,7 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2787,21 +2787,21 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>20:26</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2812,21 +2812,21 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>18:44:34</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>20:28</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2837,21 +2837,21 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>20:29</t>
+          <t>19:58</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2862,21 +2862,21 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>18:52:04</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2887,23 +2887,373 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
+          <t>18:10:41</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>110</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>90</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>20:04</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>53</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>20:13</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>62</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>20:14</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>103</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>20:25</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>74</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>20:26</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>115</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>18:44:34</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>20:28</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>104</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>18:31:18</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>20:29</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>118</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>20:43</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>92</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>20:44</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>93</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
           <t>18:52:04</t>
         </is>
       </c>
-      <c r="B102" t="inlineStr">
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>20:44</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>112</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>18:52:04</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
         <is>
           <t>20:45</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr">
+      <c r="C114" t="inlineStr">
         <is>
           <t>17X38_ROMERO</t>
         </is>
       </c>
-      <c r="D102" t="n">
+      <c r="D114" t="n">
         <v>113</v>
       </c>
-      <c r="E102" t="inlineStr">
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>21:01</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>110</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>21:02</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>111</v>
+      </c>
+      <c r="E116" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2920,7 +3270,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2938,14 +3288,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:52:04</t>
+          <t>Última actualización: 19:11:59</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 13</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -3279,23 +3629,73 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>20:43</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>92</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>18:52:04</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>20:44</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D19" t="n">
         <v>112</v>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>21:01</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>110</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3330,7 +3730,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:52:04</t>
+          <t>Última actualización: 19:11:59</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 107
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:11:59</t>
+          <t>Última actualización: 19:35:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 111</t>
+          <t>Total filas: 116</t>
         </is>
       </c>
     </row>
@@ -812,7 +812,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -822,11 +822,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -837,7 +837,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>16:50:41</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -847,11 +847,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2237,7 +2237,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2247,11 +2247,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>90</v>
+        <v>33</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>18:44:34</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2272,11 +2272,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2712,21 +2712,21 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>19:35:31</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>19:43</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2737,12 +2737,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>19:44</t>
+          <t>19:43</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2751,7 +2751,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>117</v>
+        <v>32</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,12 +2762,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>19:46</t>
+          <t>19:44</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2776,7 +2776,7 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2787,21 +2787,21 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:46</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2812,12 +2812,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2826,7 +2826,7 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2837,21 +2837,21 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>19:58</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2862,12 +2862,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:58</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2876,7 +2876,7 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2887,21 +2887,21 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,12 +2912,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2926,7 +2926,7 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2937,21 +2937,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>20:04</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2967,16 +2967,16 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:04</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,21 +2987,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>19:35:31</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>20:14</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>103</v>
+        <v>35</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3017,16 +3017,16 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>20:25</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3042,16 +3042,16 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>20:26</t>
+          <t>20:14</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3062,21 +3062,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>18:44:34</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>20:28</t>
+          <t>20:25</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3092,16 +3092,16 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>20:29</t>
+          <t>20:26</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3112,21 +3112,21 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:28</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,21 +3137,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:29</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,12 +3162,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>18:52:04</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3176,7 +3176,7 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,12 +3187,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>18:52:04</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>20:45</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3201,7 +3201,7 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,21 +3212,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>21:01</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,23 +3237,148 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
+          <t>18:52:04</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>113</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>19:35:31</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>77</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
           <t>19:11:59</t>
         </is>
       </c>
-      <c r="B116" t="inlineStr">
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>21:01</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>110</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
         <is>
           <t>21:02</t>
         </is>
       </c>
-      <c r="C116" t="inlineStr">
+      <c r="C119" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D116" t="n">
+      <c r="D119" t="n">
         <v>111</v>
       </c>
-      <c r="E116" t="inlineStr">
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>19:35:31</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>21:10</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>95</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>19:35:31</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>108</v>
+      </c>
+      <c r="E121" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3288,7 +3413,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:11:59</t>
+          <t>Última actualización: 19:35:31</t>
         </is>
       </c>
     </row>
@@ -3712,7 +3837,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3730,14 +3855,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:11:59</t>
+          <t>Última actualización: 19:35:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 13</t>
         </is>
       </c>
     </row>
@@ -4063,6 +4188,31 @@
         <v>110</v>
       </c>
       <c r="E17" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>19:35:31</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>119</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 108
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:35:31</t>
+          <t>Última actualización: 19:47:58</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 116</t>
+          <t>Total filas: 121</t>
         </is>
       </c>
     </row>
@@ -812,7 +812,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>16:50:41</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -822,11 +822,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -837,7 +837,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -847,11 +847,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -2812,21 +2812,21 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>19:47:58</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:47</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2837,12 +2837,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>17:54:43</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2851,7 +2851,7 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2862,21 +2862,21 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:54:43</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>19:58</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2887,12 +2887,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:58</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2901,7 +2901,7 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,21 +2912,21 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2937,12 +2937,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2951,7 +2951,7 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2962,21 +2962,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>19:47:58</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>20:04</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,21 +2987,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,21 +3012,21 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>19:47:58</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:02</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,21 +3037,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>20:14</t>
+          <t>20:04</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3062,21 +3062,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>19:47:58</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>20:25</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,21 +3087,21 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>19:35:31</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>20:26</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>115</v>
+        <v>35</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3112,21 +3112,21 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>18:44:34</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>20:28</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3142,16 +3142,16 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>20:29</t>
+          <t>20:14</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3167,16 +3167,16 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:25</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,21 +3187,21 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:26</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,21 +3212,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>18:52:04</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:28</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,21 +3237,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>18:52:04</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>20:45</t>
+          <t>20:29</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3262,21 +3262,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3292,16 +3292,16 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>21:01</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3312,21 +3312,21 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>21:02</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3337,21 +3337,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>20:45</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3367,18 +3367,143 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>77</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>21:01</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>110</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>21:02</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>111</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>19:47:58</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>21:06</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>79</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>19:35:31</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>21:10</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>95</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>19:35:31</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
           <t>21:23</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr">
+      <c r="C126" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D121" t="n">
+      <c r="D126" t="n">
         <v>108</v>
       </c>
-      <c r="E121" t="inlineStr">
+      <c r="E126" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3413,7 +3538,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:35:31</t>
+          <t>Última actualización: 19:47:58</t>
         </is>
       </c>
     </row>
@@ -3837,7 +3962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3855,14 +3980,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:35:31</t>
+          <t>Última actualización: 19:47:58</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 13</t>
+          <t>Total filas: 14</t>
         </is>
       </c>
     </row>
@@ -4196,23 +4321,48 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>19:47:58</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>21:33</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>106</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>19:35:31</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>21:34</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D19" t="n">
         <v>119</v>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 109
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E126"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:47:58</t>
+          <t>Última actualización: 19:54:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 121</t>
+          <t>Total filas: 125</t>
         </is>
       </c>
     </row>
@@ -812,7 +812,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>16:46:42</t>
+          <t>16:50:41</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -822,11 +822,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -837,7 +837,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>16:50:41</t>
+          <t>16:46:42</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -847,11 +847,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -2887,21 +2887,21 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>19:54:49</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>19:58</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,12 +2912,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:58</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2926,7 +2926,7 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2937,21 +2937,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2962,7 +2962,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>19:47:58</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2972,11 +2972,11 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,21 +2987,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>19:47:58</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,21 +3012,21 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>19:47:58</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>20:02</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,21 +3037,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>19:47:58</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>20:04</t>
+          <t>20:02</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3062,12 +3062,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>19:47:58</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:04</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3076,7 +3076,7 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,12 +3087,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>19:47:58</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3101,7 +3101,7 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3112,21 +3112,21 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>19:35:31</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,12 +3137,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>20:14</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3151,7 +3151,7 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,21 +3162,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>20:25</t>
+          <t>20:14</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,12 +3187,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>20:26</t>
+          <t>20:25</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3201,7 +3201,7 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,21 +3212,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>18:44:34</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>20:28</t>
+          <t>20:26</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,12 +3237,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>20:29</t>
+          <t>20:28</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3251,7 +3251,7 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3262,21 +3262,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:29</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3292,16 +3292,16 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3312,7 +3312,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>18:52:04</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3322,11 +3322,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3342,16 +3342,16 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>20:45</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3362,21 +3362,21 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:45</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3387,21 +3387,21 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>19:54:49</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>21:01</t>
+          <t>20:50</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3412,21 +3412,21 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>19:35:31</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>21:02</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3437,12 +3437,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>19:47:58</t>
+          <t>19:54:49</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>21:06</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -3451,7 +3451,7 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3462,21 +3462,21 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>21:01</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3487,23 +3487,123 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>21:02</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>111</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>19:47:58</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>21:06</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>79</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
           <t>19:35:31</t>
         </is>
       </c>
-      <c r="B126" t="inlineStr">
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>21:10</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>95</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>19:35:31</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
         <is>
           <t>21:23</t>
         </is>
       </c>
-      <c r="C126" t="inlineStr">
+      <c r="C129" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D126" t="n">
+      <c r="D129" t="n">
         <v>108</v>
       </c>
-      <c r="E126" t="inlineStr">
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>19:54:49</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>21:49</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>115</v>
+      </c>
+      <c r="E130" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3538,7 +3638,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:47:58</t>
+          <t>Última actualización: 19:54:49</t>
         </is>
       </c>
     </row>
@@ -3980,7 +4080,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:47:58</t>
+          <t>Última actualización: 19:54:49</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 110
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:54:49</t>
+          <t>Última actualización: 20:11:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 125</t>
+          <t>Total filas: 132</t>
         </is>
       </c>
     </row>
@@ -2512,7 +2512,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2522,11 +2522,11 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2537,7 +2537,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2547,11 +2547,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3137,21 +3137,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>20:11:56</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,12 +3162,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>18:31:18</t>
+          <t>20:11:56</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>20:14</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3176,7 +3176,7 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3192,16 +3192,16 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>20:25</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3217,16 +3217,16 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>20:26</t>
+          <t>20:14</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,21 +3237,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>18:44:34</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>20:28</t>
+          <t>20:25</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3267,16 +3267,16 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>20:29</t>
+          <t>20:26</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3287,21 +3287,21 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:28</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3312,21 +3312,21 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>18:31:18</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:29</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3337,21 +3337,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>18:52:04</t>
+          <t>20:11:56</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:35</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3362,21 +3362,21 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>18:52:04</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>20:45</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3387,21 +3387,21 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>19:54:49</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>20:50</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3412,21 +3412,21 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3437,21 +3437,21 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>19:54:49</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:45</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3462,21 +3462,21 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>20:11:56</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>21:01</t>
+          <t>20:49</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3487,21 +3487,21 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>19:54:49</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>21:02</t>
+          <t>20:50</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3512,21 +3512,21 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>19:47:58</t>
+          <t>19:35:31</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>21:06</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3537,12 +3537,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>19:54:49</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3551,7 +3551,7 @@
         </is>
       </c>
       <c r="D128" t="n">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,21 +3562,21 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:01</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3587,23 +3587,198 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
+          <t>19:11:59</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>21:02</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>111</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>19:47:58</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>21:06</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>79</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>19:35:31</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>21:10</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>95</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>19:35:31</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>108</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>20:11:56</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>83</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>20:11:56</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>21:48</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>97</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
           <t>19:54:49</t>
         </is>
       </c>
-      <c r="B130" t="inlineStr">
+      <c r="B136" t="inlineStr">
         <is>
           <t>21:49</t>
         </is>
       </c>
-      <c r="C130" t="inlineStr">
+      <c r="C136" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D130" t="n">
+      <c r="D136" t="n">
         <v>115</v>
       </c>
-      <c r="E130" t="inlineStr">
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>20:11:56</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>21:55</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>104</v>
+      </c>
+      <c r="E137" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3638,7 +3813,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:54:49</t>
+          <t>Última actualización: 20:11:56</t>
         </is>
       </c>
     </row>
@@ -4062,7 +4237,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4080,14 +4255,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:54:49</t>
+          <t>Última actualización: 20:11:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 14</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -4421,12 +4596,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19:47:58</t>
+          <t>20:11:56</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -4435,7 +4610,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -4446,23 +4621,48 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>19:47:58</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>21:33</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>106</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>19:35:31</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>21:34</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="D20" t="n">
         <v>119</v>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 111
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E137"/>
+  <dimension ref="A1:E149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:11:56</t>
+          <t>Última actualización: 20:32:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 132</t>
+          <t>Total filas: 144</t>
         </is>
       </c>
     </row>
@@ -1312,7 +1312,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1322,11 +1322,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1347,11 +1347,11 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2237,7 +2237,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>18:44:34</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2247,11 +2247,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>18:44:34</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2272,11 +2272,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>90</v>
+        <v>33</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2662,7 +2662,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>17:47:22</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2672,11 +2672,11 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2687,7 +2687,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>17:47:22</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2697,11 +2697,11 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>113</v>
+        <v>29</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3172,7 +3172,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3337,21 +3337,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>20:11:56</t>
+          <t>20:32:02</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>20:35</t>
+          <t>20:32</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3362,21 +3362,21 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>20:32:02</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:33</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3387,21 +3387,21 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>20:11:56</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:35</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3412,21 +3412,21 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>18:52:04</t>
+          <t>20:32:02</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:36</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>112</v>
+        <v>4</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3437,21 +3437,21 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>18:52:04</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>20:45</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3462,21 +3462,21 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>20:11:56</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>20:49</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3487,21 +3487,21 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>19:54:49</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>20:50</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3512,21 +3512,21 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:45</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3537,21 +3537,21 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>19:54:49</t>
+          <t>20:11:56</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:49</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,21 +3562,21 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>19:54:49</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>21:01</t>
+          <t>20:50</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3587,21 +3587,21 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>20:32:02</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>21:02</t>
+          <t>20:51</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,21 +3612,21 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>19:47:58</t>
+          <t>19:35:31</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>21:06</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3637,12 +3637,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>19:54:49</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3651,7 +3651,7 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3662,21 +3662,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>20:32:02</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3687,21 +3687,21 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>20:11:56</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:01</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3712,21 +3712,21 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>20:11:56</t>
+          <t>20:32:02</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>21:48</t>
+          <t>21:02</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,21 +3737,21 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>19:54:49</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>21:49</t>
+          <t>21:02</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3762,23 +3762,323 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
+          <t>19:47:58</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>21:06</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>79</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>19:35:31</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>21:10</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>95</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>19:35:31</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>108</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>21:24</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>52</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
           <t>20:11:56</t>
         </is>
       </c>
-      <c r="B137" t="inlineStr">
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>83</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>20:11:56</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>21:48</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>97</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>19:54:49</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>21:49</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>115</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>20:11:56</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
         <is>
           <t>21:55</t>
         </is>
       </c>
-      <c r="C137" t="inlineStr">
+      <c r="C144" t="inlineStr">
         <is>
           <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
-      <c r="D137" t="n">
+      <c r="D144" t="n">
         <v>104</v>
       </c>
-      <c r="E137" t="inlineStr">
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>21:56</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>84</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>22:19</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>107</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>109</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>22:26</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>114</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>22:31</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>119</v>
+      </c>
+      <c r="E149" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3795,7 +4095,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3813,14 +4113,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:11:56</t>
+          <t>Última actualización: 20:32:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -4221,6 +4521,56 @@
         <v>110</v>
       </c>
       <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>21:02</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>30</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>22:31</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>119</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4237,7 +4587,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4255,14 +4605,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:11:56</t>
+          <t>Última actualización: 20:32:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -4665,6 +5015,56 @@
       <c r="E20" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>22:13</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>101</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>22:19</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>107</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 112
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E149"/>
+  <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:32:02</t>
+          <t>Última actualización: 20:45:46</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 144</t>
+          <t>Total filas: 152</t>
         </is>
       </c>
     </row>
@@ -3537,21 +3537,21 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>20:11:56</t>
+          <t>20:45:46</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>20:49</t>
+          <t>20:46</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,21 +3562,21 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>19:54:49</t>
+          <t>20:45:46</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>20:50</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3587,12 +3587,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>20:32:02</t>
+          <t>20:11:56</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>20:51</t>
+          <t>20:49</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3601,7 +3601,7 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,12 +3612,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>19:54:49</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:50</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3626,7 +3626,7 @@
         </is>
       </c>
       <c r="D131" t="n">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3637,21 +3637,21 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>19:54:49</t>
+          <t>20:32:02</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:51</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3662,21 +3662,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>20:32:02</t>
+          <t>19:35:31</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3687,21 +3687,21 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>19:54:49</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>21:01</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3717,16 +3717,16 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>21:02</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3742,16 +3742,16 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>21:02</t>
+          <t>21:01</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3762,21 +3762,21 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>19:47:58</t>
+          <t>20:32:02</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>21:06</t>
+          <t>21:02</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,12 +3787,12 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>21:02</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -3801,7 +3801,7 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3812,21 +3812,21 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>19:35:31</t>
+          <t>19:47:58</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:06</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3837,21 +3837,21 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>20:32:02</t>
+          <t>20:45:46</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>21:24</t>
+          <t>21:06</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,21 +3862,21 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>20:11:56</t>
+          <t>19:35:31</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:10</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3887,21 +3887,21 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>20:11:56</t>
+          <t>19:35:31</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>21:48</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3912,21 +3912,21 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>19:54:49</t>
+          <t>20:32:02</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>21:49</t>
+          <t>21:24</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3937,21 +3937,21 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>20:11:56</t>
+          <t>20:45:46</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>21:55</t>
+          <t>21:30</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>104</v>
+        <v>45</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3962,21 +3962,21 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>20:32:02</t>
+          <t>20:11:56</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>21:56</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3987,21 +3987,21 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>20:32:02</t>
+          <t>20:45:46</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>22:19</t>
+          <t>21:41</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,21 +4012,21 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>20:32:02</t>
+          <t>20:11:56</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>22:21</t>
+          <t>21:48</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4037,21 +4037,21 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>20:32:02</t>
+          <t>19:54:49</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>22:26</t>
+          <t>21:49</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4062,23 +4062,223 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
+          <t>20:11:56</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>21:55</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>104</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
           <t>20:32:02</t>
         </is>
       </c>
-      <c r="B149" t="inlineStr">
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>21:56</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>84</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>20:45:46</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>22:18</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>93</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>22:19</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>107</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>109</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>20:45:46</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>22:25</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>100</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>22:26</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>114</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>20:45:46</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>105</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
         <is>
           <t>22:31</t>
         </is>
       </c>
-      <c r="C149" t="inlineStr">
+      <c r="C157" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D149" t="n">
+      <c r="D157" t="n">
         <v>119</v>
       </c>
-      <c r="E149" t="inlineStr">
+      <c r="E157" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4095,7 +4295,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4113,14 +4313,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:32:02</t>
+          <t>Última actualización: 20:45:46</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 19</t>
         </is>
       </c>
     </row>
@@ -4504,21 +4704,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>20:45:46</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>21:01</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>110</v>
+        <v>2</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -4529,12 +4729,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20:32:02</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>21:02</t>
+          <t>21:01</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -4543,7 +4743,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -4559,18 +4759,68 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>21:02</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>30</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>20:45:46</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>105</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>22:31</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="D24" t="n">
         <v>119</v>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4587,7 +4837,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4605,14 +4855,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:32:02</t>
+          <t>Última actualización: 20:45:46</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 18</t>
         </is>
       </c>
     </row>
@@ -5021,12 +5271,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20:32:02</t>
+          <t>20:45:46</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>22:13</t>
+          <t>22:12</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -5035,7 +5285,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -5051,18 +5301,43 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>22:13</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>101</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>22:19</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="D23" t="n">
         <v>107</v>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 113
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E157"/>
+  <dimension ref="A1:E158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:45:46</t>
+          <t>Última actualización: 20:52:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 152</t>
+          <t>Total filas: 153</t>
         </is>
       </c>
     </row>
@@ -3812,7 +3812,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>19:47:58</t>
+          <t>20:45:46</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -3822,11 +3822,11 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3837,7 +3837,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>20:45:46</t>
+          <t>19:47:58</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3847,11 +3847,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -4279,6 +4279,31 @@
         <v>119</v>
       </c>
       <c r="E157" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>20:52:24</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>22:49</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>117</v>
+      </c>
+      <c r="E158" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4313,7 +4338,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:45:46</t>
+          <t>Última actualización: 20:52:24</t>
         </is>
       </c>
     </row>
@@ -4855,7 +4880,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:45:46</t>
+          <t>Última actualización: 20:52:24</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 114
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-10.xlsx
+++ b/data/horarios-141-2026-01-10.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E158"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:52:24</t>
+          <t>Última actualización: 22:06:14</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 153</t>
+          <t>Total filas: 161</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>16:52:37</t>
+          <t>17:35:09</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1447,11 +1447,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1462,7 +1462,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>17:35:09</t>
+          <t>16:52:37</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1472,11 +1472,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2472,7 +2472,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -2497,7 +2497,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -2962,7 +2962,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>18:10:41</t>
+          <t>19:47:58</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2972,11 +2972,11 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>19:47:58</t>
+          <t>18:10:41</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3462,7 +3462,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>19:11:59</t>
+          <t>18:52:04</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3472,11 +3472,11 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3487,7 +3487,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>18:52:04</t>
+          <t>19:11:59</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3497,11 +3497,11 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -4187,21 +4187,21 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>20:45:46</t>
+          <t>22:06:14</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>22:25</t>
+          <t>22:21</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4212,21 +4212,21 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>20:32:02</t>
+          <t>22:06:14</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>22:26</t>
+          <t>22:22</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4242,16 +4242,16 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>22:30</t>
+          <t>22:25</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4267,16 +4267,16 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>22:31</t>
+          <t>22:26</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4287,23 +4287,223 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
+          <t>20:45:46</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>105</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>22:31</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>119</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>22:06:14</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>22:41</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>35</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
           <t>20:52:24</t>
         </is>
       </c>
-      <c r="B158" t="inlineStr">
+      <c r="B161" t="inlineStr">
         <is>
           <t>22:49</t>
         </is>
       </c>
-      <c r="C158" t="inlineStr">
+      <c r="C161" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D158" t="n">
+      <c r="D161" t="n">
         <v>117</v>
       </c>
-      <c r="E158" t="inlineStr">
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>22:06:14</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>23:06</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>60</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>22:06:14</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>23:10</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>64</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>22:06:14</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>23:19</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>73</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>22:06:14</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>23:44</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>98</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>22:06:14</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>23:49</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>103</v>
+      </c>
+      <c r="E166" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4320,7 +4520,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4338,14 +4538,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:52:24</t>
+          <t>Última actualización: 22:06:14</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 20</t>
         </is>
       </c>
     </row>
@@ -4846,6 +5046,31 @@
         <v>119</v>
       </c>
       <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>22:06:14</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>23:44</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>98</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4862,7 +5087,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4880,14 +5105,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:52:24</t>
+          <t>Última actualización: 22:06:14</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 18</t>
+          <t>Total filas: 20</t>
         </is>
       </c>
     </row>
@@ -5296,37 +5521,37 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20:45:46</t>
+          <t>22:06:14</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>22:12</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20:32:02</t>
+          <t>20:45:46</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>22:13</t>
+          <t>22:12</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -5335,7 +5560,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -5351,18 +5576,68 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>22:13</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>101</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>20:32:02</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>22:19</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D24" t="n">
         <v>107</v>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>22:06:14</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>22:23</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>17</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>